<commit_message>
I added the function to calculate means according to patterns in the variable names. However, I think returning just the variable instead of the whole dataset would be better
</commit_message>
<xml_diff>
--- a/Data/240913PRIMOCA_data.xlsx
+++ b/Data/240913PRIMOCA_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ennosgermancourse-my.sharepoint.com/personal/enno_winkler_spb-ew_de/Documents/A Fernstudium Kursmaterial/Bachelorarbeit mit bindr/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ennosgermancourse-my.sharepoint.com/personal/enno_winkler_spb-ew_de/Documents/A Fernstudium Kursmaterial/Bachelorarbeit mit bindr/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="8_{CFFF38A2-DDC3-418A-A92A-1165CA7B8675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6082BBCE-2B05-46A5-8390-1C2243299F7A}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="8_{CFFF38A2-DDC3-418A-A92A-1165CA7B8675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89750892-DB17-460E-9129-E793D344AB94}"/>
   <bookViews>
-    <workbookView xWindow="-36930" yWindow="-3870" windowWidth="28800" windowHeight="15345" xr2:uid="{18EB007D-1D64-409F-919E-E09AF6FD4925}"/>
+    <workbookView xWindow="-30045" yWindow="90" windowWidth="28800" windowHeight="15345" xr2:uid="{18EB007D-1D64-409F-919E-E09AF6FD4925}"/>
   </bookViews>
   <sheets>
     <sheet name="PRIMOCA Data set" sheetId="1" r:id="rId1"/>
@@ -1550,8 +1550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C666490-3740-4E04-A19D-0511E54407D0}">
   <dimension ref="A1:CT49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BA1" workbookViewId="0">
-      <selection activeCell="BV34" sqref="BV34"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="AE1" sqref="AE1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10838,8 +10838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CA6E932-0A6F-4492-A9D3-6FC5C8A2D811}">
   <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
There was an invisible entry in the excel sheet on line 49. I removed it and saved the new dataset.
</commit_message>
<xml_diff>
--- a/Data/240913PRIMOCA_data.xlsx
+++ b/Data/240913PRIMOCA_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ennosgermancourse-my.sharepoint.com/personal/enno_winkler_spb-ew_de/Documents/A Fernstudium Kursmaterial/Bachelorarbeit mit bindr/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ennosgermancourse-my.sharepoint.com/personal/enno_winkler_spb-ew_de/Documents/A Fernstudium Kursmaterial/Bachelorarbeit/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="8_{CFFF38A2-DDC3-418A-A92A-1165CA7B8675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89750892-DB17-460E-9129-E793D344AB94}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="8_{CFFF38A2-DDC3-418A-A92A-1165CA7B8675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5EDD8F7C-25EB-478C-B015-F8B3FDA7C885}"/>
   <bookViews>
-    <workbookView xWindow="-30045" yWindow="90" windowWidth="28800" windowHeight="15345" xr2:uid="{18EB007D-1D64-409F-919E-E09AF6FD4925}"/>
+    <workbookView xWindow="-34500" yWindow="-1440" windowWidth="28800" windowHeight="15195" xr2:uid="{18EB007D-1D64-409F-919E-E09AF6FD4925}"/>
   </bookViews>
   <sheets>
     <sheet name="PRIMOCA Data set" sheetId="1" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="307">
   <si>
     <t>Programme</t>
   </si>
@@ -995,9 +995,6 @@
   </si>
   <si>
     <t>Negative affect score  on average over assessed training sessions.</t>
-  </si>
-  <si>
-    <t>0.006269592476489028</t>
   </si>
 </sst>
 </file>
@@ -1056,15 +1053,16 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFF8F8F8"/>
+      <color rgb="FFFF0000"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="13">
@@ -1189,10 +1187,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1548,10 +1544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C666490-3740-4E04-A19D-0511E54407D0}">
-  <dimension ref="A1:CT49"/>
+  <dimension ref="A1:CT94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="AE1" sqref="AE1"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1882,7 +1878,7 @@
       <c r="H2" s="13">
         <v>6</v>
       </c>
-      <c r="I2" s="32">
+      <c r="I2" s="31">
         <v>0</v>
       </c>
       <c r="J2" s="15">
@@ -2165,7 +2161,7 @@
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
-      <c r="I3" s="32">
+      <c r="I3" s="31">
         <v>0</v>
       </c>
       <c r="J3" s="15">
@@ -2287,7 +2283,7 @@
       <c r="H4" s="13">
         <v>4</v>
       </c>
-      <c r="I4" s="32">
+      <c r="I4" s="31">
         <v>6.2695924764890297E-3</v>
       </c>
       <c r="J4" s="15">
@@ -2586,7 +2582,7 @@
       <c r="H5" s="13">
         <v>4</v>
       </c>
-      <c r="I5" s="32">
+      <c r="I5" s="31">
         <v>5.9523809523809521E-3</v>
       </c>
       <c r="J5" s="15">
@@ -2838,7 +2834,7 @@
       <c r="H6" s="13">
         <v>6</v>
       </c>
-      <c r="I6" s="32">
+      <c r="I6" s="31">
         <v>5.4844606946983544E-3</v>
       </c>
       <c r="J6" s="15">
@@ -3117,7 +3113,7 @@
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
-      <c r="I7" s="32">
+      <c r="I7" s="31">
         <v>5.1107325383304937E-3</v>
       </c>
       <c r="J7" s="15">
@@ -3317,7 +3313,7 @@
       <c r="H8" s="13">
         <v>9</v>
       </c>
-      <c r="I8" s="32">
+      <c r="I8" s="31">
         <v>3.2520325203252032E-3</v>
       </c>
       <c r="J8" s="15">
@@ -3521,7 +3517,7 @@
       <c r="H9" s="13">
         <v>5</v>
       </c>
-      <c r="I9" s="32">
+      <c r="I9" s="31">
         <v>5.9435364041604752E-3</v>
       </c>
       <c r="J9" s="15">
@@ -3807,7 +3803,7 @@
       <c r="H10" s="13">
         <v>5</v>
       </c>
-      <c r="I10" s="32">
+      <c r="I10" s="31">
         <v>0</v>
       </c>
       <c r="J10" s="15">
@@ -3961,7 +3957,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
-      <c r="I11" s="32">
+      <c r="I11" s="31">
         <v>3.7037037037037038E-3</v>
       </c>
       <c r="J11" s="15">
@@ -4083,7 +4079,7 @@
       <c r="H12" s="13">
         <v>4</v>
       </c>
-      <c r="I12" s="32">
+      <c r="I12" s="31">
         <v>4.8192771084337354E-3</v>
       </c>
       <c r="J12" s="15">
@@ -4384,7 +4380,7 @@
       <c r="H13" s="13">
         <v>4</v>
       </c>
-      <c r="I13" s="32">
+      <c r="I13" s="31">
         <v>1.2698412698412698E-2</v>
       </c>
       <c r="J13" s="15">
@@ -4606,7 +4602,7 @@
       <c r="H14" s="13">
         <v>6</v>
       </c>
-      <c r="I14" s="32">
+      <c r="I14" s="31">
         <v>5.4764512595837896E-3</v>
       </c>
       <c r="J14" s="15">
@@ -4909,7 +4905,7 @@
       <c r="H15" s="13">
         <v>4</v>
       </c>
-      <c r="I15" s="32">
+      <c r="I15" s="31">
         <v>0</v>
       </c>
       <c r="J15" s="15">
@@ -5031,7 +5027,7 @@
       <c r="H16" s="13">
         <v>5</v>
       </c>
-      <c r="I16" s="32"/>
+      <c r="I16" s="31"/>
       <c r="J16" s="15"/>
       <c r="K16" s="15"/>
       <c r="L16" s="13">
@@ -5310,7 +5306,7 @@
       <c r="F17" s="13"/>
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
-      <c r="I17" s="32">
+      <c r="I17" s="31">
         <v>2.6212319790301442E-3</v>
       </c>
       <c r="J17" s="15">
@@ -5432,7 +5428,7 @@
       <c r="H18" s="13">
         <v>4</v>
       </c>
-      <c r="I18" s="32">
+      <c r="I18" s="31">
         <v>0</v>
       </c>
       <c r="J18" s="15">
@@ -5727,7 +5723,7 @@
       <c r="H19" s="13">
         <v>6</v>
       </c>
-      <c r="I19" s="32">
+      <c r="I19" s="31">
         <v>7.1258907363420431E-3</v>
       </c>
       <c r="J19" s="15">
@@ -6030,7 +6026,7 @@
       <c r="H20" s="13">
         <v>6</v>
       </c>
-      <c r="I20" s="32">
+      <c r="I20" s="31">
         <v>0</v>
       </c>
       <c r="J20" s="15">
@@ -6319,7 +6315,7 @@
       <c r="F21" s="16"/>
       <c r="G21" s="16"/>
       <c r="H21" s="13"/>
-      <c r="I21" s="32">
+      <c r="I21" s="31">
         <v>0</v>
       </c>
       <c r="J21" s="15">
@@ -6441,7 +6437,7 @@
       <c r="H22" s="13">
         <v>5</v>
       </c>
-      <c r="I22" s="32">
+      <c r="I22" s="31">
         <v>1.2062726176115801E-3</v>
       </c>
       <c r="J22" s="15">
@@ -6744,7 +6740,7 @@
       <c r="H23" s="13">
         <v>3</v>
       </c>
-      <c r="I23" s="32">
+      <c r="I23" s="31">
         <v>6.3025210084033615E-3</v>
       </c>
       <c r="J23" s="15">
@@ -7035,7 +7031,7 @@
       <c r="H24" s="13">
         <v>9</v>
       </c>
-      <c r="I24" s="32">
+      <c r="I24" s="31">
         <v>1.4204545454545455E-3</v>
       </c>
       <c r="J24" s="15">
@@ -7293,7 +7289,7 @@
       <c r="H25" s="13">
         <v>4</v>
       </c>
-      <c r="I25" s="32">
+      <c r="I25" s="31">
         <v>0</v>
       </c>
       <c r="J25" s="15">
@@ -7501,7 +7497,7 @@
       <c r="F26" s="16"/>
       <c r="G26" s="16"/>
       <c r="H26" s="13"/>
-      <c r="I26" s="32">
+      <c r="I26" s="31">
         <v>2.4813895781637717E-3</v>
       </c>
       <c r="J26" s="15">
@@ -7623,7 +7619,7 @@
       <c r="H27" s="13">
         <v>5</v>
       </c>
-      <c r="I27" s="32">
+      <c r="I27" s="31">
         <v>3.3482142857142855E-3</v>
       </c>
       <c r="J27" s="15">
@@ -7825,7 +7821,7 @@
       <c r="H28" s="13">
         <v>3</v>
       </c>
-      <c r="I28" s="32">
+      <c r="I28" s="31">
         <v>2.843601895734597E-3</v>
       </c>
       <c r="J28" s="15">
@@ -8095,7 +8091,7 @@
       <c r="H29" s="13">
         <v>7</v>
       </c>
-      <c r="I29" s="32">
+      <c r="I29" s="31">
         <v>7.5349838536060282E-3</v>
       </c>
       <c r="J29" s="15">
@@ -8383,7 +8379,7 @@
       <c r="H30" s="13">
         <v>5</v>
       </c>
-      <c r="I30" s="32">
+      <c r="I30" s="31">
         <v>1.355421686746988E-2</v>
       </c>
       <c r="J30" s="15">
@@ -8684,7 +8680,7 @@
       <c r="H31" s="13">
         <v>6</v>
       </c>
-      <c r="I31" s="32">
+      <c r="I31" s="31">
         <v>4.61361014994233E-3</v>
       </c>
       <c r="J31" s="15">
@@ -8868,7 +8864,7 @@
       <c r="H32" s="13">
         <v>5</v>
       </c>
-      <c r="I32" s="32">
+      <c r="I32" s="31">
         <v>0</v>
       </c>
       <c r="J32" s="15">
@@ -9157,7 +9153,7 @@
       <c r="F33" s="13"/>
       <c r="G33" s="13"/>
       <c r="H33" s="13"/>
-      <c r="I33" s="32">
+      <c r="I33" s="31">
         <v>5.5248618784530384E-3</v>
       </c>
       <c r="J33" s="15">
@@ -9277,7 +9273,7 @@
       <c r="H34" s="13">
         <v>7</v>
       </c>
-      <c r="I34" s="32">
+      <c r="I34" s="31">
         <v>7.0422535211267607E-3</v>
       </c>
       <c r="J34" s="15">
@@ -9563,7 +9559,7 @@
       <c r="H35" s="13">
         <v>3</v>
       </c>
-      <c r="I35" s="32">
+      <c r="I35" s="31">
         <v>3.0581039755351682E-3</v>
       </c>
       <c r="J35" s="15">
@@ -9765,7 +9761,7 @@
       <c r="H36" s="13">
         <v>8</v>
       </c>
-      <c r="I36" s="32">
+      <c r="I36" s="31">
         <v>0</v>
       </c>
       <c r="J36" s="15">
@@ -9925,7 +9921,7 @@
       <c r="F37" s="13"/>
       <c r="G37" s="13"/>
       <c r="H37" s="13"/>
-      <c r="I37" s="32"/>
+      <c r="I37" s="31"/>
       <c r="J37" s="15"/>
       <c r="K37" s="15"/>
       <c r="L37" s="13"/>
@@ -10025,7 +10021,7 @@
       <c r="F38" s="13"/>
       <c r="G38" s="13"/>
       <c r="H38" s="13"/>
-      <c r="I38" s="32"/>
+      <c r="I38" s="31"/>
       <c r="J38" s="15"/>
       <c r="K38" s="15"/>
       <c r="L38" s="13">
@@ -10177,7 +10173,7 @@
       <c r="F39" s="13"/>
       <c r="G39" s="13"/>
       <c r="H39" s="13"/>
-      <c r="I39" s="32"/>
+      <c r="I39" s="31"/>
       <c r="J39" s="15"/>
       <c r="K39" s="15"/>
       <c r="L39" s="13">
@@ -10313,7 +10309,7 @@
       <c r="F40" s="13"/>
       <c r="G40" s="13"/>
       <c r="H40" s="13"/>
-      <c r="I40" s="32"/>
+      <c r="I40" s="31"/>
       <c r="J40" s="15"/>
       <c r="K40" s="15"/>
       <c r="L40" s="13"/>
@@ -10415,7 +10411,7 @@
       <c r="F41" s="13"/>
       <c r="G41" s="13"/>
       <c r="H41" s="13"/>
-      <c r="I41" s="32"/>
+      <c r="I41" s="31"/>
       <c r="J41" s="15"/>
       <c r="K41" s="15"/>
       <c r="L41" s="13"/>
@@ -10529,7 +10525,7 @@
       <c r="H42" s="13">
         <v>9</v>
       </c>
-      <c r="I42" s="32">
+      <c r="I42" s="31">
         <v>8.8652482269503553E-3</v>
       </c>
       <c r="J42" s="15">
@@ -10820,13 +10816,1212 @@
       <c r="CS43" s="13"/>
       <c r="CT43" s="12"/>
     </row>
+    <row r="45" spans="1:98" x14ac:dyDescent="0.25">
+      <c r="L45" s="32"/>
+      <c r="M45" s="32"/>
+      <c r="N45" s="32"/>
+      <c r="O45" s="32"/>
+      <c r="P45" s="32"/>
+      <c r="Q45" s="32"/>
+      <c r="R45" s="32"/>
+      <c r="S45" s="32"/>
+      <c r="T45" s="32"/>
+      <c r="U45" s="32"/>
+      <c r="V45" s="32"/>
+      <c r="W45" s="32"/>
+      <c r="X45" s="32"/>
+      <c r="Y45" s="32"/>
+      <c r="Z45" s="32"/>
+      <c r="AA45" s="32"/>
+      <c r="AB45" s="32"/>
+      <c r="AC45" s="32"/>
+      <c r="AD45" s="32"/>
+      <c r="AE45" s="32"/>
+      <c r="AF45" s="32"/>
+      <c r="AG45" s="32"/>
+    </row>
     <row r="46" spans="1:98" x14ac:dyDescent="0.25">
-      <c r="I46" s="31"/>
-    </row>
-    <row r="49" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I49" s="30" t="s">
-        <v>307</v>
-      </c>
+      <c r="I46" s="30"/>
+      <c r="L46" s="32"/>
+      <c r="M46" s="32"/>
+      <c r="N46" s="32"/>
+      <c r="O46" s="32"/>
+      <c r="P46" s="32"/>
+      <c r="Q46" s="32"/>
+      <c r="R46" s="32"/>
+      <c r="S46" s="32"/>
+      <c r="T46" s="32"/>
+      <c r="U46" s="32"/>
+      <c r="V46" s="32"/>
+      <c r="W46" s="32"/>
+      <c r="X46" s="32"/>
+      <c r="Y46" s="32"/>
+      <c r="Z46" s="32"/>
+      <c r="AA46" s="32"/>
+      <c r="AB46" s="32"/>
+      <c r="AC46" s="32"/>
+      <c r="AD46" s="32"/>
+      <c r="AE46" s="32"/>
+      <c r="AF46" s="32"/>
+      <c r="AG46" s="32"/>
+    </row>
+    <row r="47" spans="1:98" x14ac:dyDescent="0.25">
+      <c r="I47" s="32"/>
+      <c r="L47" s="32"/>
+      <c r="M47" s="32"/>
+      <c r="N47" s="32"/>
+      <c r="O47" s="32"/>
+      <c r="P47" s="32"/>
+      <c r="Q47" s="32"/>
+      <c r="R47" s="32"/>
+      <c r="S47" s="32"/>
+      <c r="T47" s="32"/>
+      <c r="U47" s="32"/>
+      <c r="V47" s="32"/>
+      <c r="W47" s="32"/>
+      <c r="X47" s="32"/>
+      <c r="Y47" s="32"/>
+      <c r="Z47" s="32"/>
+      <c r="AA47" s="32"/>
+      <c r="AB47" s="32"/>
+      <c r="AC47" s="32"/>
+      <c r="AD47" s="32"/>
+      <c r="AE47" s="32"/>
+      <c r="AF47" s="32"/>
+      <c r="AG47" s="32"/>
+    </row>
+    <row r="48" spans="1:98" x14ac:dyDescent="0.25">
+      <c r="I48" s="32"/>
+      <c r="L48" s="32"/>
+      <c r="M48" s="32"/>
+      <c r="N48" s="32"/>
+      <c r="O48" s="32"/>
+      <c r="P48" s="32"/>
+      <c r="Q48" s="32"/>
+      <c r="R48" s="32"/>
+      <c r="S48" s="32"/>
+      <c r="T48" s="32"/>
+      <c r="U48" s="32"/>
+      <c r="V48" s="32"/>
+      <c r="W48" s="32"/>
+      <c r="X48" s="32"/>
+      <c r="Y48" s="32"/>
+      <c r="Z48" s="32"/>
+      <c r="AA48" s="32"/>
+      <c r="AB48" s="32"/>
+      <c r="AC48" s="32"/>
+      <c r="AD48" s="32"/>
+      <c r="AE48" s="32"/>
+      <c r="AF48" s="32"/>
+      <c r="AG48" s="32"/>
+    </row>
+    <row r="49" spans="9:33" x14ac:dyDescent="0.25">
+      <c r="I49" s="30"/>
+      <c r="L49" s="32"/>
+      <c r="M49" s="32"/>
+      <c r="N49" s="32"/>
+      <c r="O49" s="32"/>
+      <c r="P49" s="32"/>
+      <c r="Q49" s="32"/>
+      <c r="R49" s="32"/>
+      <c r="S49" s="32"/>
+      <c r="T49" s="32"/>
+      <c r="U49" s="32"/>
+      <c r="V49" s="32"/>
+      <c r="W49" s="32"/>
+      <c r="X49" s="32"/>
+      <c r="Y49" s="32"/>
+      <c r="Z49" s="32"/>
+      <c r="AA49" s="32"/>
+      <c r="AB49" s="32"/>
+      <c r="AC49" s="32"/>
+      <c r="AD49" s="32"/>
+      <c r="AE49" s="32"/>
+      <c r="AF49" s="32"/>
+      <c r="AG49" s="32"/>
+    </row>
+    <row r="50" spans="9:33" x14ac:dyDescent="0.25">
+      <c r="I50" s="32"/>
+      <c r="L50" s="32"/>
+      <c r="M50" s="32"/>
+      <c r="N50" s="32"/>
+      <c r="O50" s="32"/>
+      <c r="P50" s="32"/>
+      <c r="Q50" s="32"/>
+      <c r="R50" s="32"/>
+      <c r="S50" s="32"/>
+      <c r="T50" s="32"/>
+      <c r="U50" s="32"/>
+      <c r="V50" s="32"/>
+      <c r="W50" s="32"/>
+      <c r="X50" s="32"/>
+      <c r="Y50" s="32"/>
+      <c r="Z50" s="32"/>
+      <c r="AA50" s="32"/>
+      <c r="AB50" s="32"/>
+      <c r="AC50" s="32"/>
+      <c r="AD50" s="32"/>
+      <c r="AE50" s="32"/>
+      <c r="AF50" s="32"/>
+      <c r="AG50" s="32"/>
+    </row>
+    <row r="51" spans="9:33" x14ac:dyDescent="0.25">
+      <c r="I51" s="32"/>
+      <c r="L51" s="32"/>
+      <c r="M51" s="32"/>
+      <c r="N51" s="32"/>
+      <c r="O51" s="32"/>
+      <c r="P51" s="32"/>
+      <c r="Q51" s="32"/>
+      <c r="R51" s="32"/>
+      <c r="S51" s="32"/>
+      <c r="T51" s="32"/>
+      <c r="U51" s="32"/>
+      <c r="V51" s="32"/>
+      <c r="W51" s="32"/>
+      <c r="X51" s="32"/>
+      <c r="Y51" s="32"/>
+      <c r="Z51" s="32"/>
+      <c r="AA51" s="32"/>
+      <c r="AB51" s="32"/>
+      <c r="AC51" s="32"/>
+      <c r="AD51" s="32"/>
+      <c r="AE51" s="32"/>
+      <c r="AF51" s="32"/>
+      <c r="AG51" s="32"/>
+    </row>
+    <row r="52" spans="9:33" x14ac:dyDescent="0.25">
+      <c r="I52" s="32"/>
+      <c r="L52" s="32"/>
+      <c r="M52" s="32"/>
+      <c r="N52" s="32"/>
+      <c r="O52" s="32"/>
+      <c r="P52" s="32"/>
+      <c r="Q52" s="32"/>
+      <c r="R52" s="32"/>
+      <c r="S52" s="32"/>
+      <c r="T52" s="32"/>
+      <c r="U52" s="32"/>
+      <c r="V52" s="32"/>
+      <c r="W52" s="32"/>
+      <c r="X52" s="32"/>
+      <c r="Y52" s="32"/>
+      <c r="Z52" s="32"/>
+      <c r="AA52" s="32"/>
+      <c r="AB52" s="32"/>
+      <c r="AC52" s="32"/>
+      <c r="AD52" s="32"/>
+      <c r="AE52" s="32"/>
+      <c r="AF52" s="32"/>
+      <c r="AG52" s="32"/>
+    </row>
+    <row r="53" spans="9:33" x14ac:dyDescent="0.25">
+      <c r="L53" s="32"/>
+      <c r="M53" s="32"/>
+      <c r="N53" s="32"/>
+      <c r="O53" s="32"/>
+      <c r="P53" s="32"/>
+      <c r="Q53" s="32"/>
+      <c r="R53" s="32"/>
+      <c r="S53" s="32"/>
+      <c r="T53" s="32"/>
+      <c r="U53" s="32"/>
+      <c r="V53" s="32"/>
+      <c r="W53" s="32"/>
+      <c r="X53" s="32"/>
+      <c r="Y53" s="32"/>
+      <c r="Z53" s="32"/>
+      <c r="AA53" s="32"/>
+      <c r="AB53" s="32"/>
+      <c r="AC53" s="32"/>
+      <c r="AD53" s="32"/>
+      <c r="AE53" s="32"/>
+      <c r="AF53" s="32"/>
+      <c r="AG53" s="32"/>
+    </row>
+    <row r="54" spans="9:33" x14ac:dyDescent="0.25">
+      <c r="L54" s="32"/>
+      <c r="M54" s="32"/>
+      <c r="N54" s="32"/>
+      <c r="O54" s="32"/>
+      <c r="P54" s="32"/>
+      <c r="Q54" s="32"/>
+      <c r="R54" s="32"/>
+      <c r="S54" s="32"/>
+      <c r="T54" s="32"/>
+      <c r="U54" s="32"/>
+      <c r="V54" s="32"/>
+      <c r="W54" s="32"/>
+      <c r="X54" s="32"/>
+      <c r="Y54" s="32"/>
+      <c r="Z54" s="32"/>
+      <c r="AA54" s="32"/>
+      <c r="AB54" s="32"/>
+      <c r="AC54" s="32"/>
+      <c r="AD54" s="32"/>
+      <c r="AE54" s="32"/>
+      <c r="AF54" s="32"/>
+      <c r="AG54" s="32"/>
+    </row>
+    <row r="55" spans="9:33" x14ac:dyDescent="0.25">
+      <c r="L55" s="32"/>
+      <c r="M55" s="32"/>
+      <c r="N55" s="32"/>
+      <c r="O55" s="32"/>
+      <c r="P55" s="32"/>
+      <c r="Q55" s="32"/>
+      <c r="R55" s="32"/>
+      <c r="S55" s="32"/>
+      <c r="T55" s="32"/>
+      <c r="U55" s="32"/>
+      <c r="V55" s="32"/>
+      <c r="W55" s="32"/>
+      <c r="X55" s="32"/>
+      <c r="Y55" s="32"/>
+      <c r="Z55" s="32"/>
+      <c r="AA55" s="32"/>
+      <c r="AB55" s="32"/>
+      <c r="AC55" s="32"/>
+      <c r="AD55" s="32"/>
+      <c r="AE55" s="32"/>
+      <c r="AF55" s="32"/>
+      <c r="AG55" s="32"/>
+    </row>
+    <row r="56" spans="9:33" x14ac:dyDescent="0.25">
+      <c r="L56" s="32"/>
+      <c r="M56" s="32"/>
+      <c r="N56" s="32"/>
+      <c r="O56" s="32"/>
+      <c r="P56" s="32"/>
+      <c r="Q56" s="32"/>
+      <c r="R56" s="32"/>
+      <c r="S56" s="32"/>
+      <c r="T56" s="32"/>
+      <c r="U56" s="32"/>
+      <c r="V56" s="32"/>
+      <c r="W56" s="32"/>
+      <c r="X56" s="32"/>
+      <c r="Y56" s="32"/>
+      <c r="Z56" s="32"/>
+      <c r="AA56" s="32"/>
+      <c r="AB56" s="32"/>
+      <c r="AC56" s="32"/>
+      <c r="AD56" s="32"/>
+      <c r="AE56" s="32"/>
+      <c r="AF56" s="32"/>
+      <c r="AG56" s="32"/>
+    </row>
+    <row r="57" spans="9:33" x14ac:dyDescent="0.25">
+      <c r="L57" s="32"/>
+      <c r="M57" s="32"/>
+      <c r="N57" s="32"/>
+      <c r="O57" s="32"/>
+      <c r="P57" s="32"/>
+      <c r="Q57" s="32"/>
+      <c r="R57" s="32"/>
+      <c r="S57" s="32"/>
+      <c r="T57" s="32"/>
+      <c r="U57" s="32"/>
+      <c r="V57" s="32"/>
+      <c r="W57" s="32"/>
+      <c r="X57" s="32"/>
+      <c r="Y57" s="32"/>
+      <c r="Z57" s="32"/>
+      <c r="AA57" s="32"/>
+      <c r="AB57" s="32"/>
+      <c r="AC57" s="32"/>
+      <c r="AD57" s="32"/>
+      <c r="AE57" s="32"/>
+      <c r="AF57" s="32"/>
+      <c r="AG57" s="32"/>
+    </row>
+    <row r="58" spans="9:33" x14ac:dyDescent="0.25">
+      <c r="L58" s="32"/>
+      <c r="M58" s="32"/>
+      <c r="N58" s="32"/>
+      <c r="O58" s="32"/>
+      <c r="P58" s="32"/>
+      <c r="Q58" s="32"/>
+      <c r="R58" s="32"/>
+      <c r="S58" s="32"/>
+      <c r="T58" s="32"/>
+      <c r="U58" s="32"/>
+      <c r="V58" s="32"/>
+      <c r="W58" s="32"/>
+      <c r="X58" s="32"/>
+      <c r="Y58" s="32"/>
+      <c r="Z58" s="32"/>
+      <c r="AA58" s="32"/>
+      <c r="AB58" s="32"/>
+      <c r="AC58" s="32"/>
+      <c r="AD58" s="32"/>
+      <c r="AE58" s="32"/>
+      <c r="AF58" s="32"/>
+      <c r="AG58" s="32"/>
+    </row>
+    <row r="59" spans="9:33" x14ac:dyDescent="0.25">
+      <c r="L59" s="32"/>
+      <c r="M59" s="32"/>
+      <c r="N59" s="32"/>
+      <c r="O59" s="32"/>
+      <c r="P59" s="32"/>
+      <c r="Q59" s="32"/>
+      <c r="R59" s="32"/>
+      <c r="S59" s="32"/>
+      <c r="T59" s="32"/>
+      <c r="U59" s="32"/>
+      <c r="V59" s="32"/>
+      <c r="W59" s="32"/>
+      <c r="X59" s="32"/>
+      <c r="Y59" s="32"/>
+      <c r="Z59" s="32"/>
+      <c r="AA59" s="32"/>
+      <c r="AB59" s="32"/>
+      <c r="AC59" s="32"/>
+      <c r="AD59" s="32"/>
+      <c r="AE59" s="32"/>
+      <c r="AF59" s="32"/>
+      <c r="AG59" s="32"/>
+    </row>
+    <row r="60" spans="9:33" x14ac:dyDescent="0.25">
+      <c r="L60" s="32"/>
+      <c r="M60" s="32"/>
+      <c r="N60" s="32"/>
+      <c r="O60" s="32"/>
+      <c r="P60" s="32"/>
+      <c r="Q60" s="32"/>
+      <c r="R60" s="32"/>
+      <c r="S60" s="32"/>
+      <c r="T60" s="32"/>
+      <c r="U60" s="32"/>
+      <c r="V60" s="32"/>
+      <c r="W60" s="32"/>
+      <c r="X60" s="32"/>
+      <c r="Y60" s="32"/>
+      <c r="Z60" s="32"/>
+      <c r="AA60" s="32"/>
+      <c r="AB60" s="32"/>
+      <c r="AC60" s="32"/>
+      <c r="AD60" s="32"/>
+      <c r="AE60" s="32"/>
+      <c r="AF60" s="32"/>
+      <c r="AG60" s="32"/>
+    </row>
+    <row r="61" spans="9:33" x14ac:dyDescent="0.25">
+      <c r="L61" s="32"/>
+      <c r="M61" s="32"/>
+      <c r="N61" s="32"/>
+      <c r="O61" s="32"/>
+      <c r="P61" s="32"/>
+      <c r="Q61" s="32"/>
+      <c r="R61" s="32"/>
+      <c r="S61" s="32"/>
+      <c r="T61" s="32"/>
+      <c r="U61" s="32"/>
+      <c r="V61" s="32"/>
+      <c r="W61" s="32"/>
+      <c r="X61" s="32"/>
+      <c r="Y61" s="32"/>
+      <c r="Z61" s="32"/>
+      <c r="AA61" s="32"/>
+      <c r="AB61" s="32"/>
+      <c r="AC61" s="32"/>
+      <c r="AD61" s="32"/>
+      <c r="AE61" s="32"/>
+      <c r="AF61" s="32"/>
+      <c r="AG61" s="32"/>
+    </row>
+    <row r="62" spans="9:33" x14ac:dyDescent="0.25">
+      <c r="L62" s="32"/>
+      <c r="M62" s="32"/>
+      <c r="N62" s="32"/>
+      <c r="O62" s="32"/>
+      <c r="P62" s="32"/>
+      <c r="Q62" s="32"/>
+      <c r="R62" s="32"/>
+      <c r="S62" s="32"/>
+      <c r="T62" s="32"/>
+      <c r="U62" s="32"/>
+      <c r="V62" s="32"/>
+      <c r="W62" s="32"/>
+      <c r="X62" s="32"/>
+      <c r="Y62" s="32"/>
+      <c r="Z62" s="32"/>
+      <c r="AA62" s="32"/>
+      <c r="AB62" s="32"/>
+      <c r="AC62" s="32"/>
+      <c r="AD62" s="32"/>
+      <c r="AE62" s="32"/>
+      <c r="AF62" s="32"/>
+      <c r="AG62" s="32"/>
+    </row>
+    <row r="63" spans="9:33" x14ac:dyDescent="0.25">
+      <c r="L63" s="32"/>
+      <c r="M63" s="32"/>
+      <c r="N63" s="32"/>
+      <c r="O63" s="32"/>
+      <c r="P63" s="32"/>
+      <c r="Q63" s="32"/>
+      <c r="R63" s="32"/>
+      <c r="S63" s="32"/>
+      <c r="T63" s="32"/>
+      <c r="U63" s="32"/>
+      <c r="V63" s="32"/>
+      <c r="W63" s="32"/>
+      <c r="X63" s="32"/>
+      <c r="Y63" s="32"/>
+      <c r="Z63" s="32"/>
+      <c r="AA63" s="32"/>
+      <c r="AB63" s="32"/>
+      <c r="AC63" s="32"/>
+      <c r="AD63" s="32"/>
+      <c r="AE63" s="32"/>
+      <c r="AF63" s="32"/>
+      <c r="AG63" s="32"/>
+    </row>
+    <row r="64" spans="9:33" x14ac:dyDescent="0.25">
+      <c r="L64" s="32"/>
+      <c r="M64" s="32"/>
+      <c r="N64" s="32"/>
+      <c r="O64" s="32"/>
+      <c r="P64" s="32"/>
+      <c r="Q64" s="32"/>
+      <c r="R64" s="32"/>
+      <c r="S64" s="32"/>
+      <c r="T64" s="32"/>
+      <c r="U64" s="32"/>
+      <c r="V64" s="32"/>
+      <c r="W64" s="32"/>
+      <c r="X64" s="32"/>
+      <c r="Y64" s="32"/>
+      <c r="Z64" s="32"/>
+      <c r="AA64" s="32"/>
+      <c r="AB64" s="32"/>
+      <c r="AC64" s="32"/>
+      <c r="AD64" s="32"/>
+      <c r="AE64" s="32"/>
+      <c r="AF64" s="32"/>
+      <c r="AG64" s="32"/>
+    </row>
+    <row r="65" spans="12:33" x14ac:dyDescent="0.25">
+      <c r="L65" s="32"/>
+      <c r="M65" s="32"/>
+      <c r="N65" s="32"/>
+      <c r="O65" s="32"/>
+      <c r="P65" s="32"/>
+      <c r="Q65" s="32"/>
+      <c r="R65" s="32"/>
+      <c r="S65" s="32"/>
+      <c r="T65" s="32"/>
+      <c r="U65" s="32"/>
+      <c r="V65" s="32"/>
+      <c r="W65" s="32"/>
+      <c r="X65" s="32"/>
+      <c r="Y65" s="32"/>
+      <c r="Z65" s="32"/>
+      <c r="AA65" s="32"/>
+      <c r="AB65" s="32"/>
+      <c r="AC65" s="32"/>
+      <c r="AD65" s="32"/>
+      <c r="AE65" s="32"/>
+      <c r="AF65" s="32"/>
+      <c r="AG65" s="32"/>
+    </row>
+    <row r="66" spans="12:33" x14ac:dyDescent="0.25">
+      <c r="L66" s="32"/>
+      <c r="M66" s="32"/>
+      <c r="N66" s="32"/>
+      <c r="O66" s="32"/>
+      <c r="P66" s="32"/>
+      <c r="Q66" s="32"/>
+      <c r="R66" s="32"/>
+      <c r="S66" s="32"/>
+      <c r="T66" s="32"/>
+      <c r="U66" s="32"/>
+      <c r="V66" s="32"/>
+      <c r="W66" s="32"/>
+      <c r="X66" s="32"/>
+      <c r="Y66" s="32"/>
+      <c r="Z66" s="32"/>
+      <c r="AA66" s="32"/>
+      <c r="AB66" s="32"/>
+      <c r="AC66" s="32"/>
+      <c r="AD66" s="32"/>
+      <c r="AE66" s="32"/>
+      <c r="AF66" s="32"/>
+      <c r="AG66" s="32"/>
+    </row>
+    <row r="67" spans="12:33" x14ac:dyDescent="0.25">
+      <c r="L67" s="32"/>
+      <c r="M67" s="32"/>
+      <c r="N67" s="32"/>
+      <c r="O67" s="32"/>
+      <c r="P67" s="32"/>
+      <c r="Q67" s="32"/>
+      <c r="R67" s="32"/>
+      <c r="S67" s="32"/>
+      <c r="T67" s="32"/>
+      <c r="U67" s="32"/>
+      <c r="V67" s="32"/>
+      <c r="W67" s="32"/>
+      <c r="X67" s="32"/>
+      <c r="Y67" s="32"/>
+      <c r="Z67" s="32"/>
+      <c r="AA67" s="32"/>
+      <c r="AB67" s="32"/>
+      <c r="AC67" s="32"/>
+      <c r="AD67" s="32"/>
+      <c r="AE67" s="32"/>
+      <c r="AF67" s="32"/>
+      <c r="AG67" s="32"/>
+    </row>
+    <row r="68" spans="12:33" x14ac:dyDescent="0.25">
+      <c r="L68" s="32"/>
+      <c r="M68" s="32"/>
+      <c r="N68" s="32"/>
+      <c r="O68" s="32"/>
+      <c r="P68" s="32"/>
+      <c r="Q68" s="32"/>
+      <c r="R68" s="32"/>
+      <c r="S68" s="32"/>
+      <c r="T68" s="32"/>
+      <c r="U68" s="32"/>
+      <c r="V68" s="32"/>
+      <c r="W68" s="32"/>
+      <c r="X68" s="32"/>
+      <c r="Y68" s="32"/>
+      <c r="Z68" s="32"/>
+      <c r="AA68" s="32"/>
+      <c r="AB68" s="32"/>
+      <c r="AC68" s="32"/>
+      <c r="AD68" s="32"/>
+      <c r="AE68" s="32"/>
+      <c r="AF68" s="32"/>
+      <c r="AG68" s="32"/>
+    </row>
+    <row r="69" spans="12:33" x14ac:dyDescent="0.25">
+      <c r="L69" s="32"/>
+      <c r="M69" s="32"/>
+      <c r="N69" s="32"/>
+      <c r="O69" s="32"/>
+      <c r="P69" s="32"/>
+      <c r="Q69" s="32"/>
+      <c r="R69" s="32"/>
+      <c r="S69" s="32"/>
+      <c r="T69" s="32"/>
+      <c r="U69" s="32"/>
+      <c r="V69" s="32"/>
+      <c r="W69" s="32"/>
+      <c r="X69" s="32"/>
+      <c r="Y69" s="32"/>
+      <c r="Z69" s="32"/>
+      <c r="AA69" s="32"/>
+      <c r="AB69" s="32"/>
+      <c r="AC69" s="32"/>
+      <c r="AD69" s="32"/>
+      <c r="AE69" s="32"/>
+      <c r="AF69" s="32"/>
+      <c r="AG69" s="32"/>
+    </row>
+    <row r="70" spans="12:33" x14ac:dyDescent="0.25">
+      <c r="L70" s="32"/>
+      <c r="M70" s="32"/>
+      <c r="N70" s="32"/>
+      <c r="O70" s="32"/>
+      <c r="P70" s="32"/>
+      <c r="Q70" s="32"/>
+      <c r="R70" s="32"/>
+      <c r="S70" s="32"/>
+      <c r="T70" s="32"/>
+      <c r="U70" s="32"/>
+      <c r="V70" s="32"/>
+      <c r="W70" s="32"/>
+      <c r="X70" s="32"/>
+      <c r="Y70" s="32"/>
+      <c r="Z70" s="32"/>
+      <c r="AA70" s="32"/>
+      <c r="AB70" s="32"/>
+      <c r="AC70" s="32"/>
+      <c r="AD70" s="32"/>
+      <c r="AE70" s="32"/>
+      <c r="AF70" s="32"/>
+      <c r="AG70" s="32"/>
+    </row>
+    <row r="71" spans="12:33" x14ac:dyDescent="0.25">
+      <c r="L71" s="32"/>
+      <c r="M71" s="32"/>
+      <c r="N71" s="32"/>
+      <c r="O71" s="32"/>
+      <c r="P71" s="32"/>
+      <c r="Q71" s="32"/>
+      <c r="R71" s="32"/>
+      <c r="S71" s="32"/>
+      <c r="T71" s="32"/>
+      <c r="U71" s="32"/>
+      <c r="V71" s="32"/>
+      <c r="W71" s="32"/>
+      <c r="X71" s="32"/>
+      <c r="Y71" s="32"/>
+      <c r="Z71" s="32"/>
+      <c r="AA71" s="32"/>
+      <c r="AB71" s="32"/>
+      <c r="AC71" s="32"/>
+      <c r="AD71" s="32"/>
+      <c r="AE71" s="32"/>
+      <c r="AF71" s="32"/>
+      <c r="AG71" s="32"/>
+    </row>
+    <row r="72" spans="12:33" x14ac:dyDescent="0.25">
+      <c r="L72" s="32"/>
+      <c r="M72" s="32"/>
+      <c r="N72" s="32"/>
+      <c r="O72" s="32"/>
+      <c r="P72" s="32"/>
+      <c r="Q72" s="32"/>
+      <c r="R72" s="32"/>
+      <c r="S72" s="32"/>
+      <c r="T72" s="32"/>
+      <c r="U72" s="32"/>
+      <c r="V72" s="32"/>
+      <c r="W72" s="32"/>
+      <c r="X72" s="32"/>
+      <c r="Y72" s="32"/>
+      <c r="Z72" s="32"/>
+      <c r="AA72" s="32"/>
+      <c r="AB72" s="32"/>
+      <c r="AC72" s="32"/>
+      <c r="AD72" s="32"/>
+      <c r="AE72" s="32"/>
+      <c r="AF72" s="32"/>
+      <c r="AG72" s="32"/>
+    </row>
+    <row r="73" spans="12:33" x14ac:dyDescent="0.25">
+      <c r="L73" s="32"/>
+      <c r="M73" s="32"/>
+      <c r="N73" s="32"/>
+      <c r="O73" s="32"/>
+      <c r="P73" s="32"/>
+      <c r="Q73" s="32"/>
+      <c r="R73" s="32"/>
+      <c r="S73" s="32"/>
+      <c r="T73" s="32"/>
+      <c r="U73" s="32"/>
+      <c r="V73" s="32"/>
+      <c r="W73" s="32"/>
+      <c r="X73" s="32"/>
+      <c r="Y73" s="32"/>
+      <c r="Z73" s="32"/>
+      <c r="AA73" s="32"/>
+      <c r="AB73" s="32"/>
+      <c r="AC73" s="32"/>
+      <c r="AD73" s="32"/>
+      <c r="AE73" s="32"/>
+      <c r="AF73" s="32"/>
+      <c r="AG73" s="32"/>
+    </row>
+    <row r="74" spans="12:33" x14ac:dyDescent="0.25">
+      <c r="L74" s="32"/>
+      <c r="M74" s="32"/>
+      <c r="N74" s="32"/>
+      <c r="O74" s="32"/>
+      <c r="P74" s="32"/>
+      <c r="Q74" s="32"/>
+      <c r="R74" s="32"/>
+      <c r="S74" s="32"/>
+      <c r="T74" s="32"/>
+      <c r="U74" s="32"/>
+      <c r="V74" s="32"/>
+      <c r="W74" s="32"/>
+      <c r="X74" s="32"/>
+      <c r="Y74" s="32"/>
+      <c r="Z74" s="32"/>
+      <c r="AA74" s="32"/>
+      <c r="AB74" s="32"/>
+      <c r="AC74" s="32"/>
+      <c r="AD74" s="32"/>
+      <c r="AE74" s="32"/>
+      <c r="AF74" s="32"/>
+      <c r="AG74" s="32"/>
+    </row>
+    <row r="75" spans="12:33" x14ac:dyDescent="0.25">
+      <c r="L75" s="32"/>
+      <c r="M75" s="32"/>
+      <c r="N75" s="32"/>
+      <c r="O75" s="32"/>
+      <c r="P75" s="32"/>
+      <c r="Q75" s="32"/>
+      <c r="R75" s="32"/>
+      <c r="S75" s="32"/>
+      <c r="T75" s="32"/>
+      <c r="U75" s="32"/>
+      <c r="V75" s="32"/>
+      <c r="W75" s="32"/>
+      <c r="X75" s="32"/>
+      <c r="Y75" s="32"/>
+      <c r="Z75" s="32"/>
+      <c r="AA75" s="32"/>
+      <c r="AB75" s="32"/>
+      <c r="AC75" s="32"/>
+      <c r="AD75" s="32"/>
+      <c r="AE75" s="32"/>
+      <c r="AF75" s="32"/>
+      <c r="AG75" s="32"/>
+    </row>
+    <row r="76" spans="12:33" x14ac:dyDescent="0.25">
+      <c r="L76" s="32"/>
+      <c r="M76" s="32"/>
+      <c r="N76" s="32"/>
+      <c r="O76" s="32"/>
+      <c r="P76" s="32"/>
+      <c r="Q76" s="32"/>
+      <c r="R76" s="32"/>
+      <c r="S76" s="32"/>
+      <c r="T76" s="32"/>
+      <c r="U76" s="32"/>
+      <c r="V76" s="32"/>
+      <c r="W76" s="32"/>
+      <c r="X76" s="32"/>
+      <c r="Y76" s="32"/>
+      <c r="Z76" s="32"/>
+      <c r="AA76" s="32"/>
+      <c r="AB76" s="32"/>
+      <c r="AC76" s="32"/>
+      <c r="AD76" s="32"/>
+      <c r="AE76" s="32"/>
+      <c r="AF76" s="32"/>
+      <c r="AG76" s="32"/>
+    </row>
+    <row r="77" spans="12:33" x14ac:dyDescent="0.25">
+      <c r="L77" s="32"/>
+      <c r="M77" s="32"/>
+      <c r="N77" s="32"/>
+      <c r="O77" s="32"/>
+      <c r="P77" s="32"/>
+      <c r="Q77" s="32"/>
+      <c r="R77" s="32"/>
+      <c r="S77" s="32"/>
+      <c r="T77" s="32"/>
+      <c r="U77" s="32"/>
+      <c r="V77" s="32"/>
+      <c r="W77" s="32"/>
+      <c r="X77" s="32"/>
+      <c r="Y77" s="32"/>
+      <c r="Z77" s="32"/>
+      <c r="AA77" s="32"/>
+      <c r="AB77" s="32"/>
+      <c r="AC77" s="32"/>
+      <c r="AD77" s="32"/>
+      <c r="AE77" s="32"/>
+      <c r="AF77" s="32"/>
+      <c r="AG77" s="32"/>
+    </row>
+    <row r="78" spans="12:33" x14ac:dyDescent="0.25">
+      <c r="L78" s="32"/>
+      <c r="M78" s="32"/>
+      <c r="N78" s="32"/>
+      <c r="O78" s="32"/>
+      <c r="P78" s="32"/>
+      <c r="Q78" s="32"/>
+      <c r="R78" s="32"/>
+      <c r="S78" s="32"/>
+      <c r="T78" s="32"/>
+      <c r="U78" s="32"/>
+      <c r="V78" s="32"/>
+      <c r="W78" s="32"/>
+      <c r="X78" s="32"/>
+      <c r="Y78" s="32"/>
+      <c r="Z78" s="32"/>
+      <c r="AA78" s="32"/>
+      <c r="AB78" s="32"/>
+      <c r="AC78" s="32"/>
+      <c r="AD78" s="32"/>
+      <c r="AE78" s="32"/>
+      <c r="AF78" s="32"/>
+      <c r="AG78" s="32"/>
+    </row>
+    <row r="79" spans="12:33" x14ac:dyDescent="0.25">
+      <c r="L79" s="32"/>
+      <c r="M79" s="32"/>
+      <c r="N79" s="32"/>
+      <c r="O79" s="32"/>
+      <c r="P79" s="32"/>
+      <c r="Q79" s="32"/>
+      <c r="R79" s="32"/>
+      <c r="S79" s="32"/>
+      <c r="T79" s="32"/>
+      <c r="U79" s="32"/>
+      <c r="V79" s="32"/>
+      <c r="W79" s="32"/>
+      <c r="X79" s="32"/>
+      <c r="Y79" s="32"/>
+      <c r="Z79" s="32"/>
+      <c r="AA79" s="32"/>
+      <c r="AB79" s="32"/>
+      <c r="AC79" s="32"/>
+      <c r="AD79" s="32"/>
+      <c r="AE79" s="32"/>
+      <c r="AF79" s="32"/>
+      <c r="AG79" s="32"/>
+    </row>
+    <row r="80" spans="12:33" x14ac:dyDescent="0.25">
+      <c r="L80" s="32"/>
+      <c r="M80" s="32"/>
+      <c r="N80" s="32"/>
+      <c r="O80" s="32"/>
+      <c r="P80" s="32"/>
+      <c r="Q80" s="32"/>
+      <c r="R80" s="32"/>
+      <c r="S80" s="32"/>
+      <c r="T80" s="32"/>
+      <c r="U80" s="32"/>
+      <c r="V80" s="32"/>
+      <c r="W80" s="32"/>
+      <c r="X80" s="32"/>
+      <c r="Y80" s="32"/>
+      <c r="Z80" s="32"/>
+      <c r="AA80" s="32"/>
+      <c r="AB80" s="32"/>
+      <c r="AC80" s="32"/>
+      <c r="AD80" s="32"/>
+      <c r="AE80" s="32"/>
+      <c r="AF80" s="32"/>
+      <c r="AG80" s="32"/>
+    </row>
+    <row r="81" spans="12:33" x14ac:dyDescent="0.25">
+      <c r="L81" s="32"/>
+      <c r="M81" s="32"/>
+      <c r="N81" s="32"/>
+      <c r="O81" s="32"/>
+      <c r="P81" s="32"/>
+      <c r="Q81" s="32"/>
+      <c r="R81" s="32"/>
+      <c r="S81" s="32"/>
+      <c r="T81" s="32"/>
+      <c r="U81" s="32"/>
+      <c r="V81" s="32"/>
+      <c r="W81" s="32"/>
+      <c r="X81" s="32"/>
+      <c r="Y81" s="32"/>
+      <c r="Z81" s="32"/>
+      <c r="AA81" s="32"/>
+      <c r="AB81" s="32"/>
+      <c r="AC81" s="32"/>
+      <c r="AD81" s="32"/>
+      <c r="AE81" s="32"/>
+      <c r="AF81" s="32"/>
+      <c r="AG81" s="32"/>
+    </row>
+    <row r="82" spans="12:33" x14ac:dyDescent="0.25">
+      <c r="L82" s="32"/>
+      <c r="M82" s="32"/>
+      <c r="N82" s="32"/>
+      <c r="O82" s="32"/>
+      <c r="P82" s="32"/>
+      <c r="Q82" s="32"/>
+      <c r="R82" s="32"/>
+      <c r="S82" s="32"/>
+      <c r="T82" s="32"/>
+      <c r="U82" s="32"/>
+      <c r="V82" s="32"/>
+      <c r="W82" s="32"/>
+      <c r="X82" s="32"/>
+      <c r="Y82" s="32"/>
+      <c r="Z82" s="32"/>
+      <c r="AA82" s="32"/>
+      <c r="AB82" s="32"/>
+      <c r="AC82" s="32"/>
+      <c r="AD82" s="32"/>
+      <c r="AE82" s="32"/>
+      <c r="AF82" s="32"/>
+      <c r="AG82" s="32"/>
+    </row>
+    <row r="83" spans="12:33" x14ac:dyDescent="0.25">
+      <c r="L83" s="32"/>
+      <c r="M83" s="32"/>
+      <c r="N83" s="32"/>
+      <c r="O83" s="32"/>
+      <c r="P83" s="32"/>
+      <c r="Q83" s="32"/>
+      <c r="R83" s="32"/>
+      <c r="S83" s="32"/>
+      <c r="T83" s="32"/>
+      <c r="U83" s="32"/>
+      <c r="V83" s="32"/>
+      <c r="W83" s="32"/>
+      <c r="X83" s="32"/>
+      <c r="Y83" s="32"/>
+      <c r="Z83" s="32"/>
+      <c r="AA83" s="32"/>
+      <c r="AB83" s="32"/>
+      <c r="AC83" s="32"/>
+      <c r="AD83" s="32"/>
+      <c r="AE83" s="32"/>
+      <c r="AF83" s="32"/>
+      <c r="AG83" s="32"/>
+    </row>
+    <row r="84" spans="12:33" x14ac:dyDescent="0.25">
+      <c r="L84" s="32"/>
+      <c r="M84" s="32"/>
+      <c r="N84" s="32"/>
+      <c r="O84" s="32"/>
+      <c r="P84" s="32"/>
+      <c r="Q84" s="32"/>
+      <c r="R84" s="32"/>
+      <c r="S84" s="32"/>
+      <c r="T84" s="32"/>
+      <c r="U84" s="32"/>
+      <c r="V84" s="32"/>
+      <c r="W84" s="32"/>
+      <c r="X84" s="32"/>
+      <c r="Y84" s="32"/>
+      <c r="Z84" s="32"/>
+      <c r="AA84" s="32"/>
+      <c r="AB84" s="32"/>
+      <c r="AC84" s="32"/>
+      <c r="AD84" s="32"/>
+      <c r="AE84" s="32"/>
+      <c r="AF84" s="32"/>
+      <c r="AG84" s="32"/>
+    </row>
+    <row r="85" spans="12:33" x14ac:dyDescent="0.25">
+      <c r="L85" s="32"/>
+      <c r="M85" s="32"/>
+      <c r="N85" s="32"/>
+      <c r="O85" s="32"/>
+      <c r="P85" s="32"/>
+      <c r="Q85" s="32"/>
+      <c r="R85" s="32"/>
+      <c r="S85" s="32"/>
+      <c r="T85" s="32"/>
+      <c r="U85" s="32"/>
+      <c r="V85" s="32"/>
+      <c r="W85" s="32"/>
+      <c r="X85" s="32"/>
+      <c r="Y85" s="32"/>
+      <c r="Z85" s="32"/>
+      <c r="AA85" s="32"/>
+      <c r="AB85" s="32"/>
+      <c r="AC85" s="32"/>
+      <c r="AD85" s="32"/>
+      <c r="AE85" s="32"/>
+      <c r="AF85" s="32"/>
+      <c r="AG85" s="32"/>
+    </row>
+    <row r="86" spans="12:33" x14ac:dyDescent="0.25">
+      <c r="L86" s="32"/>
+      <c r="M86" s="32"/>
+      <c r="N86" s="32"/>
+      <c r="O86" s="32"/>
+      <c r="P86" s="32"/>
+      <c r="Q86" s="32"/>
+      <c r="R86" s="32"/>
+      <c r="S86" s="32"/>
+      <c r="T86" s="32"/>
+      <c r="U86" s="32"/>
+      <c r="V86" s="32"/>
+      <c r="W86" s="32"/>
+      <c r="X86" s="32"/>
+      <c r="Y86" s="32"/>
+      <c r="Z86" s="32"/>
+      <c r="AA86" s="32"/>
+      <c r="AB86" s="32"/>
+      <c r="AC86" s="32"/>
+      <c r="AD86" s="32"/>
+      <c r="AE86" s="32"/>
+      <c r="AF86" s="32"/>
+      <c r="AG86" s="32"/>
+    </row>
+    <row r="87" spans="12:33" x14ac:dyDescent="0.25">
+      <c r="L87" s="32"/>
+      <c r="M87" s="32"/>
+      <c r="N87" s="32"/>
+      <c r="O87" s="32"/>
+      <c r="P87" s="32"/>
+      <c r="Q87" s="32"/>
+      <c r="R87" s="32"/>
+      <c r="S87" s="32"/>
+      <c r="T87" s="32"/>
+      <c r="U87" s="32"/>
+      <c r="V87" s="32"/>
+      <c r="W87" s="32"/>
+      <c r="X87" s="32"/>
+      <c r="Y87" s="32"/>
+      <c r="Z87" s="32"/>
+      <c r="AA87" s="32"/>
+      <c r="AB87" s="32"/>
+      <c r="AC87" s="32"/>
+      <c r="AD87" s="32"/>
+      <c r="AE87" s="32"/>
+      <c r="AF87" s="32"/>
+      <c r="AG87" s="32"/>
+    </row>
+    <row r="88" spans="12:33" x14ac:dyDescent="0.25">
+      <c r="L88" s="32"/>
+      <c r="M88" s="32"/>
+      <c r="N88" s="32"/>
+      <c r="O88" s="32"/>
+      <c r="P88" s="32"/>
+      <c r="Q88" s="32"/>
+      <c r="R88" s="32"/>
+      <c r="S88" s="32"/>
+      <c r="T88" s="32"/>
+      <c r="U88" s="32"/>
+      <c r="V88" s="32"/>
+      <c r="W88" s="32"/>
+      <c r="X88" s="32"/>
+      <c r="Y88" s="32"/>
+      <c r="Z88" s="32"/>
+      <c r="AA88" s="32"/>
+      <c r="AB88" s="32"/>
+      <c r="AC88" s="32"/>
+      <c r="AD88" s="32"/>
+      <c r="AE88" s="32"/>
+      <c r="AF88" s="32"/>
+      <c r="AG88" s="32"/>
+    </row>
+    <row r="89" spans="12:33" x14ac:dyDescent="0.25">
+      <c r="L89" s="32"/>
+      <c r="M89" s="32"/>
+      <c r="N89" s="32"/>
+      <c r="O89" s="32"/>
+      <c r="P89" s="32"/>
+      <c r="Q89" s="32"/>
+      <c r="R89" s="32"/>
+      <c r="S89" s="32"/>
+      <c r="T89" s="32"/>
+      <c r="U89" s="32"/>
+      <c r="V89" s="32"/>
+      <c r="W89" s="32"/>
+      <c r="X89" s="32"/>
+      <c r="Y89" s="32"/>
+      <c r="Z89" s="32"/>
+      <c r="AA89" s="32"/>
+      <c r="AB89" s="32"/>
+      <c r="AC89" s="32"/>
+      <c r="AD89" s="32"/>
+      <c r="AE89" s="32"/>
+      <c r="AF89" s="32"/>
+      <c r="AG89" s="32"/>
+    </row>
+    <row r="90" spans="12:33" x14ac:dyDescent="0.25">
+      <c r="L90" s="32"/>
+      <c r="M90" s="32"/>
+      <c r="N90" s="32"/>
+      <c r="O90" s="32"/>
+      <c r="P90" s="32"/>
+      <c r="Q90" s="32"/>
+      <c r="R90" s="32"/>
+      <c r="S90" s="32"/>
+      <c r="T90" s="32"/>
+      <c r="U90" s="32"/>
+      <c r="V90" s="32"/>
+      <c r="W90" s="32"/>
+      <c r="X90" s="32"/>
+      <c r="Y90" s="32"/>
+      <c r="Z90" s="32"/>
+      <c r="AA90" s="32"/>
+      <c r="AB90" s="32"/>
+      <c r="AC90" s="32"/>
+      <c r="AD90" s="32"/>
+      <c r="AE90" s="32"/>
+      <c r="AF90" s="32"/>
+      <c r="AG90" s="32"/>
+    </row>
+    <row r="91" spans="12:33" x14ac:dyDescent="0.25">
+      <c r="L91" s="32"/>
+      <c r="M91" s="32"/>
+      <c r="N91" s="32"/>
+      <c r="O91" s="32"/>
+      <c r="P91" s="32"/>
+      <c r="Q91" s="32"/>
+      <c r="R91" s="32"/>
+      <c r="S91" s="32"/>
+      <c r="T91" s="32"/>
+      <c r="U91" s="32"/>
+      <c r="V91" s="32"/>
+      <c r="W91" s="32"/>
+      <c r="X91" s="32"/>
+      <c r="Y91" s="32"/>
+      <c r="Z91" s="32"/>
+      <c r="AA91" s="32"/>
+      <c r="AB91" s="32"/>
+      <c r="AC91" s="32"/>
+      <c r="AD91" s="32"/>
+      <c r="AE91" s="32"/>
+      <c r="AF91" s="32"/>
+      <c r="AG91" s="32"/>
+    </row>
+    <row r="92" spans="12:33" x14ac:dyDescent="0.25">
+      <c r="L92" s="32"/>
+      <c r="M92" s="32"/>
+      <c r="N92" s="32"/>
+      <c r="O92" s="32"/>
+      <c r="P92" s="32"/>
+      <c r="Q92" s="32"/>
+      <c r="R92" s="32"/>
+      <c r="S92" s="32"/>
+      <c r="T92" s="32"/>
+      <c r="U92" s="32"/>
+      <c r="V92" s="32"/>
+      <c r="W92" s="32"/>
+      <c r="X92" s="32"/>
+      <c r="Y92" s="32"/>
+      <c r="Z92" s="32"/>
+      <c r="AA92" s="32"/>
+      <c r="AB92" s="32"/>
+      <c r="AC92" s="32"/>
+      <c r="AD92" s="32"/>
+      <c r="AE92" s="32"/>
+      <c r="AF92" s="32"/>
+      <c r="AG92" s="32"/>
+    </row>
+    <row r="93" spans="12:33" x14ac:dyDescent="0.25">
+      <c r="L93" s="32"/>
+      <c r="M93" s="32"/>
+      <c r="N93" s="32"/>
+      <c r="O93" s="32"/>
+      <c r="P93" s="32"/>
+      <c r="Q93" s="32"/>
+      <c r="R93" s="32"/>
+      <c r="S93" s="32"/>
+      <c r="T93" s="32"/>
+      <c r="U93" s="32"/>
+      <c r="V93" s="32"/>
+      <c r="W93" s="32"/>
+      <c r="X93" s="32"/>
+      <c r="Y93" s="32"/>
+      <c r="Z93" s="32"/>
+      <c r="AA93" s="32"/>
+      <c r="AB93" s="32"/>
+      <c r="AC93" s="32"/>
+      <c r="AD93" s="32"/>
+      <c r="AE93" s="32"/>
+      <c r="AF93" s="32"/>
+      <c r="AG93" s="32"/>
+    </row>
+    <row r="94" spans="12:33" x14ac:dyDescent="0.25">
+      <c r="L94" s="32"/>
+      <c r="M94" s="32"/>
+      <c r="N94" s="32"/>
+      <c r="O94" s="32"/>
+      <c r="P94" s="32"/>
+      <c r="Q94" s="32"/>
+      <c r="R94" s="32"/>
+      <c r="S94" s="32"/>
+      <c r="T94" s="32"/>
+      <c r="U94" s="32"/>
+      <c r="V94" s="32"/>
+      <c r="W94" s="32"/>
+      <c r="X94" s="32"/>
+      <c r="Y94" s="32"/>
+      <c r="Z94" s="32"/>
+      <c r="AA94" s="32"/>
+      <c r="AB94" s="32"/>
+      <c r="AC94" s="32"/>
+      <c r="AD94" s="32"/>
+      <c r="AE94" s="32"/>
+      <c r="AF94" s="32"/>
+      <c r="AG94" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Messung zu Physischer Aktivität hinzugefügt
</commit_message>
<xml_diff>
--- a/Data/240913PRIMOCA_data.xlsx
+++ b/Data/240913PRIMOCA_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28719"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ennosgermancourse-my.sharepoint.com/personal/enno_winkler_spb-ew_de/Documents/A Fernstudium Kursmaterial/Bachelorarbeit/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="8_{CFFF38A2-DDC3-418A-A92A-1165CA7B8675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5EDD8F7C-25EB-478C-B015-F8B3FDA7C885}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="8_{CFFF38A2-DDC3-418A-A92A-1165CA7B8675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9FD57101-6CDD-4ADA-93BF-A7DE4EDB0316}"/>
   <bookViews>
     <workbookView xWindow="-34500" yWindow="-1440" windowWidth="28800" windowHeight="15195" xr2:uid="{18EB007D-1D64-409F-919E-E09AF6FD4925}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="PRIMOCA Data set" sheetId="1" r:id="rId1"/>
     <sheet name="PRIMOCA Code book" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191028" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1005,7 +1005,7 @@
     <numFmt numFmtId="164" formatCode="0.0000000000000000"/>
     <numFmt numFmtId="165" formatCode="0.00000000000000000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1191,7 +1191,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1546,18 +1546,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C666490-3740-4E04-A19D-0511E54407D0}">
   <dimension ref="A1:CT94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="9" max="9" width="61" customWidth="1"/>
+    <col min="10" max="10" width="43.42578125" customWidth="1"/>
+    <col min="11" max="11" width="49.7109375" customWidth="1"/>
     <col min="74" max="74" width="17.5703125" customWidth="1"/>
     <col min="75" max="75" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:98" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1853,7 +1855,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:98" ht="15.75">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -2150,7 +2152,7 @@
       </c>
       <c r="CT2" s="12"/>
     </row>
-    <row r="3" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:98" ht="15.75">
       <c r="A3" s="12">
         <v>2</v>
       </c>
@@ -2258,7 +2260,7 @@
       <c r="CS3" s="13"/>
       <c r="CT3" s="12"/>
     </row>
-    <row r="4" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:98" ht="15.75">
       <c r="A4" s="12">
         <v>1</v>
       </c>
@@ -2557,7 +2559,7 @@
       </c>
       <c r="CT4" s="12"/>
     </row>
-    <row r="5" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:98" ht="15.75">
       <c r="A5" s="12">
         <v>1</v>
       </c>
@@ -2811,7 +2813,7 @@
       <c r="CS5" s="13"/>
       <c r="CT5" s="12"/>
     </row>
-    <row r="6" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:98" ht="15.75">
       <c r="A6" s="12">
         <v>1</v>
       </c>
@@ -3104,7 +3106,7 @@
       </c>
       <c r="CT6" s="12"/>
     </row>
-    <row r="7" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:98" ht="15.75">
       <c r="A7" s="12"/>
       <c r="B7" s="13"/>
       <c r="C7" s="12"/>
@@ -3290,7 +3292,7 @@
       <c r="CS7" s="13"/>
       <c r="CT7" s="12"/>
     </row>
-    <row r="8" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:98" ht="15.75">
       <c r="A8" s="12">
         <v>1</v>
       </c>
@@ -3492,7 +3494,7 @@
       <c r="CS8" s="13"/>
       <c r="CT8" s="12"/>
     </row>
-    <row r="9" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:98" ht="15.75">
       <c r="A9" s="12">
         <v>1</v>
       </c>
@@ -3780,7 +3782,7 @@
       </c>
       <c r="CT9" s="12"/>
     </row>
-    <row r="10" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:98" ht="15.75">
       <c r="A10" s="12">
         <v>1</v>
       </c>
@@ -3946,7 +3948,7 @@
       <c r="CS10" s="13"/>
       <c r="CT10" s="12"/>
     </row>
-    <row r="11" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:98" ht="15.75">
       <c r="A11" s="12">
         <v>2</v>
       </c>
@@ -4054,7 +4056,7 @@
       <c r="CS11" s="13"/>
       <c r="CT11" s="12"/>
     </row>
-    <row r="12" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:98" ht="15.75">
       <c r="A12" s="12">
         <v>1</v>
       </c>
@@ -4355,7 +4357,7 @@
       </c>
       <c r="CT12" s="12"/>
     </row>
-    <row r="13" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:98" ht="15.75">
       <c r="A13" s="12">
         <v>1</v>
       </c>
@@ -4577,7 +4579,7 @@
       <c r="CS13" s="13"/>
       <c r="CT13" s="12"/>
     </row>
-    <row r="14" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:98" ht="15.75">
       <c r="A14" s="12">
         <v>1</v>
       </c>
@@ -4880,7 +4882,7 @@
       </c>
       <c r="CT14" s="12"/>
     </row>
-    <row r="15" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:98" ht="15.75">
       <c r="A15" s="12">
         <v>1</v>
       </c>
@@ -5002,7 +5004,7 @@
       <c r="CS15" s="13"/>
       <c r="CT15" s="12"/>
     </row>
-    <row r="16" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:98" ht="15.75">
       <c r="A16" s="12">
         <v>1</v>
       </c>
@@ -5295,7 +5297,7 @@
       </c>
       <c r="CT16" s="12"/>
     </row>
-    <row r="17" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:98" ht="15.75">
       <c r="A17" s="12">
         <v>2</v>
       </c>
@@ -5403,7 +5405,7 @@
       <c r="CS17" s="13"/>
       <c r="CT17" s="12"/>
     </row>
-    <row r="18" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:98" ht="15.75">
       <c r="A18" s="12">
         <v>1</v>
       </c>
@@ -5700,7 +5702,7 @@
       </c>
       <c r="CT18" s="12"/>
     </row>
-    <row r="19" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:98" ht="15.75">
       <c r="A19" s="12">
         <v>1</v>
       </c>
@@ -6001,7 +6003,7 @@
       </c>
       <c r="CT19" s="12"/>
     </row>
-    <row r="20" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:98" ht="15.75">
       <c r="A20" s="12">
         <v>1</v>
       </c>
@@ -6304,7 +6306,7 @@
       </c>
       <c r="CT20" s="12"/>
     </row>
-    <row r="21" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:98" ht="15.75">
       <c r="A21" s="12">
         <v>2</v>
       </c>
@@ -6412,7 +6414,7 @@
       <c r="CS21" s="13"/>
       <c r="CT21" s="12"/>
     </row>
-    <row r="22" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:98" ht="15.75">
       <c r="A22" s="12">
         <v>1</v>
       </c>
@@ -6715,7 +6717,7 @@
       </c>
       <c r="CT22" s="12"/>
     </row>
-    <row r="23" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:98" ht="15.75">
       <c r="A23" s="12">
         <v>1</v>
       </c>
@@ -7006,7 +7008,7 @@
       </c>
       <c r="CT23" s="12"/>
     </row>
-    <row r="24" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:98" ht="15.75">
       <c r="A24" s="12">
         <v>1</v>
       </c>
@@ -7264,7 +7266,7 @@
       <c r="CS24" s="13"/>
       <c r="CT24" s="12"/>
     </row>
-    <row r="25" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:98" ht="15.75">
       <c r="A25" s="12">
         <v>1</v>
       </c>
@@ -7486,7 +7488,7 @@
       <c r="CS25" s="13"/>
       <c r="CT25" s="12"/>
     </row>
-    <row r="26" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:98" ht="15.75">
       <c r="A26" s="12">
         <v>2</v>
       </c>
@@ -7594,7 +7596,7 @@
       <c r="CS26" s="13"/>
       <c r="CT26" s="12"/>
     </row>
-    <row r="27" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:98" ht="15.75">
       <c r="A27" s="12">
         <v>1</v>
       </c>
@@ -7798,7 +7800,7 @@
       <c r="CS27" s="13"/>
       <c r="CT27" s="12"/>
     </row>
-    <row r="28" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:98" ht="15.75">
       <c r="A28" s="12">
         <v>1</v>
       </c>
@@ -8066,7 +8068,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="29" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:98" ht="15.75">
       <c r="A29" s="12">
         <v>1</v>
       </c>
@@ -8354,7 +8356,7 @@
       </c>
       <c r="CT29" s="12"/>
     </row>
-    <row r="30" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:98" ht="15.75">
       <c r="A30" s="12">
         <v>1</v>
       </c>
@@ -8657,7 +8659,7 @@
       </c>
       <c r="CT30" s="12"/>
     </row>
-    <row r="31" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:98" ht="15.75">
       <c r="A31" s="12">
         <v>1</v>
       </c>
@@ -8839,7 +8841,7 @@
       <c r="CS31" s="13"/>
       <c r="CT31" s="12"/>
     </row>
-    <row r="32" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:98" ht="15.75">
       <c r="A32" s="12">
         <v>1</v>
       </c>
@@ -9142,7 +9144,7 @@
       </c>
       <c r="CT32" s="12"/>
     </row>
-    <row r="33" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:98" ht="15.75">
       <c r="A33" s="12">
         <v>2</v>
       </c>
@@ -9250,7 +9252,7 @@
       <c r="CS33" s="13"/>
       <c r="CT33" s="12"/>
     </row>
-    <row r="34" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:98" ht="15.75">
       <c r="A34" s="12">
         <v>1</v>
       </c>
@@ -9536,7 +9538,7 @@
       </c>
       <c r="CT34" s="12"/>
     </row>
-    <row r="35" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:98" ht="15.75">
       <c r="A35" s="12">
         <v>1</v>
       </c>
@@ -9736,7 +9738,7 @@
       <c r="CS35" s="13"/>
       <c r="CT35" s="12"/>
     </row>
-    <row r="36" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:98" ht="15.75">
       <c r="A36" s="12">
         <v>1</v>
       </c>
@@ -9910,7 +9912,7 @@
       <c r="CS36" s="13"/>
       <c r="CT36" s="12"/>
     </row>
-    <row r="37" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:98" ht="15.75">
       <c r="A37" s="12">
         <v>2</v>
       </c>
@@ -10012,7 +10014,7 @@
       <c r="CS37" s="13"/>
       <c r="CT37" s="12"/>
     </row>
-    <row r="38" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:98" ht="15.75">
       <c r="A38" s="12"/>
       <c r="B38" s="13"/>
       <c r="C38" s="12"/>
@@ -10164,7 +10166,7 @@
       <c r="CS38" s="13"/>
       <c r="CT38" s="12"/>
     </row>
-    <row r="39" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:98" ht="15.75">
       <c r="A39" s="12"/>
       <c r="B39" s="13"/>
       <c r="C39" s="12"/>
@@ -10298,7 +10300,7 @@
       <c r="CS39" s="13"/>
       <c r="CT39" s="12"/>
     </row>
-    <row r="40" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:98" ht="15.75">
       <c r="A40" s="12">
         <v>2</v>
       </c>
@@ -10400,7 +10402,7 @@
       <c r="CS40" s="13"/>
       <c r="CT40" s="12"/>
     </row>
-    <row r="41" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:98" ht="15.75">
       <c r="A41" s="12">
         <v>2</v>
       </c>
@@ -10502,7 +10504,7 @@
       <c r="CS41" s="13"/>
       <c r="CT41" s="12"/>
     </row>
-    <row r="42" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:98" ht="15.75">
       <c r="A42" s="12">
         <v>1</v>
       </c>
@@ -10700,7 +10702,7 @@
       <c r="CS42" s="13"/>
       <c r="CT42" s="12"/>
     </row>
-    <row r="43" spans="1:98" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:98" ht="15.75">
       <c r="A43" s="12"/>
       <c r="B43" s="13"/>
       <c r="C43" s="12"/>
@@ -10816,7 +10818,7 @@
       <c r="CS43" s="13"/>
       <c r="CT43" s="12"/>
     </row>
-    <row r="45" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:98">
       <c r="L45" s="32"/>
       <c r="M45" s="32"/>
       <c r="N45" s="32"/>
@@ -10840,7 +10842,7 @@
       <c r="AF45" s="32"/>
       <c r="AG45" s="32"/>
     </row>
-    <row r="46" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:98">
       <c r="I46" s="30"/>
       <c r="L46" s="32"/>
       <c r="M46" s="32"/>
@@ -10865,7 +10867,7 @@
       <c r="AF46" s="32"/>
       <c r="AG46" s="32"/>
     </row>
-    <row r="47" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:98">
       <c r="I47" s="32"/>
       <c r="L47" s="32"/>
       <c r="M47" s="32"/>
@@ -10890,7 +10892,7 @@
       <c r="AF47" s="32"/>
       <c r="AG47" s="32"/>
     </row>
-    <row r="48" spans="1:98" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:98">
       <c r="I48" s="32"/>
       <c r="L48" s="32"/>
       <c r="M48" s="32"/>
@@ -10915,7 +10917,7 @@
       <c r="AF48" s="32"/>
       <c r="AG48" s="32"/>
     </row>
-    <row r="49" spans="9:33" x14ac:dyDescent="0.25">
+    <row r="49" spans="9:33">
       <c r="I49" s="30"/>
       <c r="L49" s="32"/>
       <c r="M49" s="32"/>
@@ -10940,7 +10942,7 @@
       <c r="AF49" s="32"/>
       <c r="AG49" s="32"/>
     </row>
-    <row r="50" spans="9:33" x14ac:dyDescent="0.25">
+    <row r="50" spans="9:33">
       <c r="I50" s="32"/>
       <c r="L50" s="32"/>
       <c r="M50" s="32"/>
@@ -10965,7 +10967,7 @@
       <c r="AF50" s="32"/>
       <c r="AG50" s="32"/>
     </row>
-    <row r="51" spans="9:33" x14ac:dyDescent="0.25">
+    <row r="51" spans="9:33">
       <c r="I51" s="32"/>
       <c r="L51" s="32"/>
       <c r="M51" s="32"/>
@@ -10990,7 +10992,7 @@
       <c r="AF51" s="32"/>
       <c r="AG51" s="32"/>
     </row>
-    <row r="52" spans="9:33" x14ac:dyDescent="0.25">
+    <row r="52" spans="9:33">
       <c r="I52" s="32"/>
       <c r="L52" s="32"/>
       <c r="M52" s="32"/>
@@ -11015,7 +11017,7 @@
       <c r="AF52" s="32"/>
       <c r="AG52" s="32"/>
     </row>
-    <row r="53" spans="9:33" x14ac:dyDescent="0.25">
+    <row r="53" spans="9:33">
       <c r="L53" s="32"/>
       <c r="M53" s="32"/>
       <c r="N53" s="32"/>
@@ -11039,7 +11041,7 @@
       <c r="AF53" s="32"/>
       <c r="AG53" s="32"/>
     </row>
-    <row r="54" spans="9:33" x14ac:dyDescent="0.25">
+    <row r="54" spans="9:33">
       <c r="L54" s="32"/>
       <c r="M54" s="32"/>
       <c r="N54" s="32"/>
@@ -11063,7 +11065,7 @@
       <c r="AF54" s="32"/>
       <c r="AG54" s="32"/>
     </row>
-    <row r="55" spans="9:33" x14ac:dyDescent="0.25">
+    <row r="55" spans="9:33">
       <c r="L55" s="32"/>
       <c r="M55" s="32"/>
       <c r="N55" s="32"/>
@@ -11087,7 +11089,7 @@
       <c r="AF55" s="32"/>
       <c r="AG55" s="32"/>
     </row>
-    <row r="56" spans="9:33" x14ac:dyDescent="0.25">
+    <row r="56" spans="9:33">
       <c r="L56" s="32"/>
       <c r="M56" s="32"/>
       <c r="N56" s="32"/>
@@ -11111,7 +11113,7 @@
       <c r="AF56" s="32"/>
       <c r="AG56" s="32"/>
     </row>
-    <row r="57" spans="9:33" x14ac:dyDescent="0.25">
+    <row r="57" spans="9:33">
       <c r="L57" s="32"/>
       <c r="M57" s="32"/>
       <c r="N57" s="32"/>
@@ -11135,7 +11137,7 @@
       <c r="AF57" s="32"/>
       <c r="AG57" s="32"/>
     </row>
-    <row r="58" spans="9:33" x14ac:dyDescent="0.25">
+    <row r="58" spans="9:33">
       <c r="L58" s="32"/>
       <c r="M58" s="32"/>
       <c r="N58" s="32"/>
@@ -11159,7 +11161,7 @@
       <c r="AF58" s="32"/>
       <c r="AG58" s="32"/>
     </row>
-    <row r="59" spans="9:33" x14ac:dyDescent="0.25">
+    <row r="59" spans="9:33">
       <c r="L59" s="32"/>
       <c r="M59" s="32"/>
       <c r="N59" s="32"/>
@@ -11183,7 +11185,7 @@
       <c r="AF59" s="32"/>
       <c r="AG59" s="32"/>
     </row>
-    <row r="60" spans="9:33" x14ac:dyDescent="0.25">
+    <row r="60" spans="9:33">
       <c r="L60" s="32"/>
       <c r="M60" s="32"/>
       <c r="N60" s="32"/>
@@ -11207,7 +11209,7 @@
       <c r="AF60" s="32"/>
       <c r="AG60" s="32"/>
     </row>
-    <row r="61" spans="9:33" x14ac:dyDescent="0.25">
+    <row r="61" spans="9:33">
       <c r="L61" s="32"/>
       <c r="M61" s="32"/>
       <c r="N61" s="32"/>
@@ -11231,7 +11233,7 @@
       <c r="AF61" s="32"/>
       <c r="AG61" s="32"/>
     </row>
-    <row r="62" spans="9:33" x14ac:dyDescent="0.25">
+    <row r="62" spans="9:33">
       <c r="L62" s="32"/>
       <c r="M62" s="32"/>
       <c r="N62" s="32"/>
@@ -11255,7 +11257,7 @@
       <c r="AF62" s="32"/>
       <c r="AG62" s="32"/>
     </row>
-    <row r="63" spans="9:33" x14ac:dyDescent="0.25">
+    <row r="63" spans="9:33">
       <c r="L63" s="32"/>
       <c r="M63" s="32"/>
       <c r="N63" s="32"/>
@@ -11279,7 +11281,7 @@
       <c r="AF63" s="32"/>
       <c r="AG63" s="32"/>
     </row>
-    <row r="64" spans="9:33" x14ac:dyDescent="0.25">
+    <row r="64" spans="9:33">
       <c r="L64" s="32"/>
       <c r="M64" s="32"/>
       <c r="N64" s="32"/>
@@ -11303,7 +11305,7 @@
       <c r="AF64" s="32"/>
       <c r="AG64" s="32"/>
     </row>
-    <row r="65" spans="12:33" x14ac:dyDescent="0.25">
+    <row r="65" spans="12:33">
       <c r="L65" s="32"/>
       <c r="M65" s="32"/>
       <c r="N65" s="32"/>
@@ -11327,7 +11329,7 @@
       <c r="AF65" s="32"/>
       <c r="AG65" s="32"/>
     </row>
-    <row r="66" spans="12:33" x14ac:dyDescent="0.25">
+    <row r="66" spans="12:33">
       <c r="L66" s="32"/>
       <c r="M66" s="32"/>
       <c r="N66" s="32"/>
@@ -11351,7 +11353,7 @@
       <c r="AF66" s="32"/>
       <c r="AG66" s="32"/>
     </row>
-    <row r="67" spans="12:33" x14ac:dyDescent="0.25">
+    <row r="67" spans="12:33">
       <c r="L67" s="32"/>
       <c r="M67" s="32"/>
       <c r="N67" s="32"/>
@@ -11375,7 +11377,7 @@
       <c r="AF67" s="32"/>
       <c r="AG67" s="32"/>
     </row>
-    <row r="68" spans="12:33" x14ac:dyDescent="0.25">
+    <row r="68" spans="12:33">
       <c r="L68" s="32"/>
       <c r="M68" s="32"/>
       <c r="N68" s="32"/>
@@ -11399,7 +11401,7 @@
       <c r="AF68" s="32"/>
       <c r="AG68" s="32"/>
     </row>
-    <row r="69" spans="12:33" x14ac:dyDescent="0.25">
+    <row r="69" spans="12:33">
       <c r="L69" s="32"/>
       <c r="M69" s="32"/>
       <c r="N69" s="32"/>
@@ -11423,7 +11425,7 @@
       <c r="AF69" s="32"/>
       <c r="AG69" s="32"/>
     </row>
-    <row r="70" spans="12:33" x14ac:dyDescent="0.25">
+    <row r="70" spans="12:33">
       <c r="L70" s="32"/>
       <c r="M70" s="32"/>
       <c r="N70" s="32"/>
@@ -11447,7 +11449,7 @@
       <c r="AF70" s="32"/>
       <c r="AG70" s="32"/>
     </row>
-    <row r="71" spans="12:33" x14ac:dyDescent="0.25">
+    <row r="71" spans="12:33">
       <c r="L71" s="32"/>
       <c r="M71" s="32"/>
       <c r="N71" s="32"/>
@@ -11471,7 +11473,7 @@
       <c r="AF71" s="32"/>
       <c r="AG71" s="32"/>
     </row>
-    <row r="72" spans="12:33" x14ac:dyDescent="0.25">
+    <row r="72" spans="12:33">
       <c r="L72" s="32"/>
       <c r="M72" s="32"/>
       <c r="N72" s="32"/>
@@ -11495,7 +11497,7 @@
       <c r="AF72" s="32"/>
       <c r="AG72" s="32"/>
     </row>
-    <row r="73" spans="12:33" x14ac:dyDescent="0.25">
+    <row r="73" spans="12:33">
       <c r="L73" s="32"/>
       <c r="M73" s="32"/>
       <c r="N73" s="32"/>
@@ -11519,7 +11521,7 @@
       <c r="AF73" s="32"/>
       <c r="AG73" s="32"/>
     </row>
-    <row r="74" spans="12:33" x14ac:dyDescent="0.25">
+    <row r="74" spans="12:33">
       <c r="L74" s="32"/>
       <c r="M74" s="32"/>
       <c r="N74" s="32"/>
@@ -11543,7 +11545,7 @@
       <c r="AF74" s="32"/>
       <c r="AG74" s="32"/>
     </row>
-    <row r="75" spans="12:33" x14ac:dyDescent="0.25">
+    <row r="75" spans="12:33">
       <c r="L75" s="32"/>
       <c r="M75" s="32"/>
       <c r="N75" s="32"/>
@@ -11567,7 +11569,7 @@
       <c r="AF75" s="32"/>
       <c r="AG75" s="32"/>
     </row>
-    <row r="76" spans="12:33" x14ac:dyDescent="0.25">
+    <row r="76" spans="12:33">
       <c r="L76" s="32"/>
       <c r="M76" s="32"/>
       <c r="N76" s="32"/>
@@ -11591,7 +11593,7 @@
       <c r="AF76" s="32"/>
       <c r="AG76" s="32"/>
     </row>
-    <row r="77" spans="12:33" x14ac:dyDescent="0.25">
+    <row r="77" spans="12:33">
       <c r="L77" s="32"/>
       <c r="M77" s="32"/>
       <c r="N77" s="32"/>
@@ -11615,7 +11617,7 @@
       <c r="AF77" s="32"/>
       <c r="AG77" s="32"/>
     </row>
-    <row r="78" spans="12:33" x14ac:dyDescent="0.25">
+    <row r="78" spans="12:33">
       <c r="L78" s="32"/>
       <c r="M78" s="32"/>
       <c r="N78" s="32"/>
@@ -11639,7 +11641,7 @@
       <c r="AF78" s="32"/>
       <c r="AG78" s="32"/>
     </row>
-    <row r="79" spans="12:33" x14ac:dyDescent="0.25">
+    <row r="79" spans="12:33">
       <c r="L79" s="32"/>
       <c r="M79" s="32"/>
       <c r="N79" s="32"/>
@@ -11663,7 +11665,7 @@
       <c r="AF79" s="32"/>
       <c r="AG79" s="32"/>
     </row>
-    <row r="80" spans="12:33" x14ac:dyDescent="0.25">
+    <row r="80" spans="12:33">
       <c r="L80" s="32"/>
       <c r="M80" s="32"/>
       <c r="N80" s="32"/>
@@ -11687,7 +11689,7 @@
       <c r="AF80" s="32"/>
       <c r="AG80" s="32"/>
     </row>
-    <row r="81" spans="12:33" x14ac:dyDescent="0.25">
+    <row r="81" spans="12:33">
       <c r="L81" s="32"/>
       <c r="M81" s="32"/>
       <c r="N81" s="32"/>
@@ -11711,7 +11713,7 @@
       <c r="AF81" s="32"/>
       <c r="AG81" s="32"/>
     </row>
-    <row r="82" spans="12:33" x14ac:dyDescent="0.25">
+    <row r="82" spans="12:33">
       <c r="L82" s="32"/>
       <c r="M82" s="32"/>
       <c r="N82" s="32"/>
@@ -11735,7 +11737,7 @@
       <c r="AF82" s="32"/>
       <c r="AG82" s="32"/>
     </row>
-    <row r="83" spans="12:33" x14ac:dyDescent="0.25">
+    <row r="83" spans="12:33">
       <c r="L83" s="32"/>
       <c r="M83" s="32"/>
       <c r="N83" s="32"/>
@@ -11759,7 +11761,7 @@
       <c r="AF83" s="32"/>
       <c r="AG83" s="32"/>
     </row>
-    <row r="84" spans="12:33" x14ac:dyDescent="0.25">
+    <row r="84" spans="12:33">
       <c r="L84" s="32"/>
       <c r="M84" s="32"/>
       <c r="N84" s="32"/>
@@ -11783,7 +11785,7 @@
       <c r="AF84" s="32"/>
       <c r="AG84" s="32"/>
     </row>
-    <row r="85" spans="12:33" x14ac:dyDescent="0.25">
+    <row r="85" spans="12:33">
       <c r="L85" s="32"/>
       <c r="M85" s="32"/>
       <c r="N85" s="32"/>
@@ -11807,7 +11809,7 @@
       <c r="AF85" s="32"/>
       <c r="AG85" s="32"/>
     </row>
-    <row r="86" spans="12:33" x14ac:dyDescent="0.25">
+    <row r="86" spans="12:33">
       <c r="L86" s="32"/>
       <c r="M86" s="32"/>
       <c r="N86" s="32"/>
@@ -11831,7 +11833,7 @@
       <c r="AF86" s="32"/>
       <c r="AG86" s="32"/>
     </row>
-    <row r="87" spans="12:33" x14ac:dyDescent="0.25">
+    <row r="87" spans="12:33">
       <c r="L87" s="32"/>
       <c r="M87" s="32"/>
       <c r="N87" s="32"/>
@@ -11855,7 +11857,7 @@
       <c r="AF87" s="32"/>
       <c r="AG87" s="32"/>
     </row>
-    <row r="88" spans="12:33" x14ac:dyDescent="0.25">
+    <row r="88" spans="12:33">
       <c r="L88" s="32"/>
       <c r="M88" s="32"/>
       <c r="N88" s="32"/>
@@ -11879,7 +11881,7 @@
       <c r="AF88" s="32"/>
       <c r="AG88" s="32"/>
     </row>
-    <row r="89" spans="12:33" x14ac:dyDescent="0.25">
+    <row r="89" spans="12:33">
       <c r="L89" s="32"/>
       <c r="M89" s="32"/>
       <c r="N89" s="32"/>
@@ -11903,7 +11905,7 @@
       <c r="AF89" s="32"/>
       <c r="AG89" s="32"/>
     </row>
-    <row r="90" spans="12:33" x14ac:dyDescent="0.25">
+    <row r="90" spans="12:33">
       <c r="L90" s="32"/>
       <c r="M90" s="32"/>
       <c r="N90" s="32"/>
@@ -11927,7 +11929,7 @@
       <c r="AF90" s="32"/>
       <c r="AG90" s="32"/>
     </row>
-    <row r="91" spans="12:33" x14ac:dyDescent="0.25">
+    <row r="91" spans="12:33">
       <c r="L91" s="32"/>
       <c r="M91" s="32"/>
       <c r="N91" s="32"/>
@@ -11951,7 +11953,7 @@
       <c r="AF91" s="32"/>
       <c r="AG91" s="32"/>
     </row>
-    <row r="92" spans="12:33" x14ac:dyDescent="0.25">
+    <row r="92" spans="12:33">
       <c r="L92" s="32"/>
       <c r="M92" s="32"/>
       <c r="N92" s="32"/>
@@ -11975,7 +11977,7 @@
       <c r="AF92" s="32"/>
       <c r="AG92" s="32"/>
     </row>
-    <row r="93" spans="12:33" x14ac:dyDescent="0.25">
+    <row r="93" spans="12:33">
       <c r="L93" s="32"/>
       <c r="M93" s="32"/>
       <c r="N93" s="32"/>
@@ -11999,7 +12001,7 @@
       <c r="AF93" s="32"/>
       <c r="AG93" s="32"/>
     </row>
-    <row r="94" spans="12:33" x14ac:dyDescent="0.25">
+    <row r="94" spans="12:33">
       <c r="L94" s="32"/>
       <c r="M94" s="32"/>
       <c r="N94" s="32"/>
@@ -12037,14 +12039,14 @@
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
     <col min="2" max="2" width="93.28515625" customWidth="1"/>
     <col min="3" max="3" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75">
       <c r="A1" s="11" t="s">
         <v>142</v>
       </c>
@@ -12061,7 +12063,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15.75">
       <c r="A2" s="12" t="s">
         <v>146</v>
       </c>
@@ -12074,7 +12076,7 @@
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
     </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="15.75">
       <c r="A3" s="12" t="s">
         <v>149</v>
       </c>
@@ -12089,7 +12091,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15.75">
       <c r="A4" s="12" t="s">
         <v>0</v>
       </c>
@@ -12104,7 +12106,7 @@
       </c>
       <c r="E4" s="12"/>
     </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15.75">
       <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
@@ -12119,7 +12121,7 @@
       </c>
       <c r="E5" s="12"/>
     </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15.75">
       <c r="A6" s="12" t="s">
         <v>2</v>
       </c>
@@ -12134,7 +12136,7 @@
       </c>
       <c r="E6" s="12"/>
     </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15.75">
       <c r="A7" s="12" t="s">
         <v>3</v>
       </c>
@@ -12149,7 +12151,7 @@
       </c>
       <c r="E7" s="12"/>
     </row>
-    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="15.75">
       <c r="A8" s="12" t="s">
         <v>4</v>
       </c>
@@ -12164,7 +12166,7 @@
       </c>
       <c r="E8" s="12"/>
     </row>
-    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="15.75">
       <c r="A9" s="12" t="s">
         <v>5</v>
       </c>
@@ -12179,7 +12181,7 @@
       </c>
       <c r="E9" s="12"/>
     </row>
-    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="15.75">
       <c r="A10" s="12" t="s">
         <v>6</v>
       </c>
@@ -12194,7 +12196,7 @@
       </c>
       <c r="E10" s="12"/>
     </row>
-    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="15.75">
       <c r="A11" s="12" t="s">
         <v>7</v>
       </c>
@@ -12209,7 +12211,7 @@
       </c>
       <c r="E11" s="12"/>
     </row>
-    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="15.75">
       <c r="A12" s="12" t="s">
         <v>8</v>
       </c>
@@ -12226,7 +12228,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="15.75">
       <c r="A13" s="12" t="s">
         <v>9</v>
       </c>
@@ -12243,7 +12245,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="15.75">
       <c r="A14" s="12" t="s">
         <v>10</v>
       </c>
@@ -12260,7 +12262,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="15.75">
       <c r="A15" s="12" t="s">
         <v>11</v>
       </c>
@@ -12277,7 +12279,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="15.75">
       <c r="A16" s="12" t="s">
         <v>12</v>
       </c>
@@ -12294,7 +12296,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="15.75">
       <c r="A17" s="12" t="s">
         <v>13</v>
       </c>
@@ -12311,7 +12313,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="15.75">
       <c r="A18" s="12" t="s">
         <v>14</v>
       </c>
@@ -12328,7 +12330,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="15.75">
       <c r="A19" s="12" t="s">
         <v>15</v>
       </c>
@@ -12345,7 +12347,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="15.75">
       <c r="A20" s="12" t="s">
         <v>16</v>
       </c>
@@ -12362,7 +12364,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="15.75">
       <c r="A21" s="12" t="s">
         <v>17</v>
       </c>
@@ -12377,7 +12379,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="15.75">
       <c r="A22" s="12" t="s">
         <v>18</v>
       </c>
@@ -12392,7 +12394,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="15.75">
       <c r="A23" s="12" t="s">
         <v>19</v>
       </c>
@@ -12407,7 +12409,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="15.75">
       <c r="A24" s="12" t="s">
         <v>20</v>
       </c>
@@ -12422,7 +12424,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="15.75">
       <c r="A25" s="12" t="s">
         <v>21</v>
       </c>
@@ -12437,7 +12439,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="15.75">
       <c r="A26" s="12" t="s">
         <v>22</v>
       </c>
@@ -12452,7 +12454,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="15.75">
       <c r="A27" s="12" t="s">
         <v>23</v>
       </c>
@@ -12469,7 +12471,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="15.75">
       <c r="A28" s="12" t="s">
         <v>24</v>
       </c>
@@ -12486,7 +12488,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="15.75">
       <c r="A29" s="12" t="s">
         <v>25</v>
       </c>
@@ -12503,7 +12505,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="15.75">
       <c r="A30" s="12" t="s">
         <v>26</v>
       </c>
@@ -12520,7 +12522,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="15.75">
       <c r="A31" s="12" t="s">
         <v>27</v>
       </c>
@@ -12537,7 +12539,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="15.75">
       <c r="A32" s="12" t="s">
         <v>28</v>
       </c>
@@ -12554,7 +12556,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="15.75">
       <c r="A33" s="12" t="s">
         <v>29</v>
       </c>
@@ -12571,7 +12573,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="15.75">
       <c r="A34" s="12" t="s">
         <v>30</v>
       </c>
@@ -12588,7 +12590,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="15.75">
       <c r="A35" s="12" t="s">
         <v>31</v>
       </c>
@@ -12605,7 +12607,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="15.75">
       <c r="A36" s="12" t="s">
         <v>32</v>
       </c>
@@ -12622,7 +12624,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="15.75">
       <c r="A37" s="12" t="s">
         <v>33</v>
       </c>
@@ -12639,7 +12641,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="15.75">
       <c r="A38" s="12" t="s">
         <v>34</v>
       </c>
@@ -12654,7 +12656,7 @@
       </c>
       <c r="E38" s="12"/>
     </row>
-    <row r="39" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="15.75">
       <c r="A39" s="12" t="s">
         <v>35</v>
       </c>
@@ -12669,7 +12671,7 @@
       </c>
       <c r="E39" s="12"/>
     </row>
-    <row r="40" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="15.75">
       <c r="A40" s="12" t="s">
         <v>36</v>
       </c>
@@ -12684,7 +12686,7 @@
       </c>
       <c r="E40" s="12"/>
     </row>
-    <row r="41" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="15.75">
       <c r="A41" s="12" t="s">
         <v>37</v>
       </c>
@@ -12699,7 +12701,7 @@
       </c>
       <c r="E41" s="12"/>
     </row>
-    <row r="42" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="15.75">
       <c r="A42" s="12" t="s">
         <v>38</v>
       </c>
@@ -12714,7 +12716,7 @@
       </c>
       <c r="E42" s="12"/>
     </row>
-    <row r="43" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="15.75">
       <c r="A43" s="12" t="s">
         <v>39</v>
       </c>
@@ -12731,7 +12733,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="15.75">
       <c r="A44" s="12" t="s">
         <v>40</v>
       </c>
@@ -12748,7 +12750,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="15.75">
       <c r="A45" s="12" t="s">
         <v>41</v>
       </c>
@@ -12765,7 +12767,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="15.75">
       <c r="A46" s="12" t="s">
         <v>42</v>
       </c>
@@ -12782,7 +12784,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="15.75">
       <c r="A47" s="12" t="s">
         <v>43</v>
       </c>
@@ -12797,7 +12799,7 @@
       </c>
       <c r="E47" s="12"/>
     </row>
-    <row r="48" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="15.75">
       <c r="A48" s="12" t="s">
         <v>44</v>
       </c>
@@ -12812,7 +12814,7 @@
       </c>
       <c r="E48" s="12"/>
     </row>
-    <row r="49" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="15.75">
       <c r="A49" s="12" t="s">
         <v>45</v>
       </c>
@@ -12827,7 +12829,7 @@
       </c>
       <c r="E49" s="12"/>
     </row>
-    <row r="50" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="15.75">
       <c r="A50" s="12" t="s">
         <v>46</v>
       </c>
@@ -12842,7 +12844,7 @@
       </c>
       <c r="E50" s="12"/>
     </row>
-    <row r="51" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="15.75">
       <c r="A51" s="12" t="s">
         <v>47</v>
       </c>
@@ -12857,7 +12859,7 @@
       </c>
       <c r="E51" s="12"/>
     </row>
-    <row r="52" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="15.75">
       <c r="A52" s="12" t="s">
         <v>48</v>
       </c>
@@ -12874,7 +12876,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="15.75">
       <c r="A53" s="12" t="s">
         <v>49</v>
       </c>
@@ -12891,7 +12893,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="15.75">
       <c r="A54" s="12" t="s">
         <v>50</v>
       </c>
@@ -12908,7 +12910,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="15.75">
       <c r="A55" s="12" t="s">
         <v>51</v>
       </c>
@@ -12925,7 +12927,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" ht="15.75">
       <c r="A56" s="12" t="s">
         <v>52</v>
       </c>
@@ -12940,7 +12942,7 @@
       </c>
       <c r="E56" s="12"/>
     </row>
-    <row r="57" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="15.75">
       <c r="A57" s="12" t="s">
         <v>53</v>
       </c>
@@ -12955,7 +12957,7 @@
       </c>
       <c r="E57" s="12"/>
     </row>
-    <row r="58" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" ht="15.75">
       <c r="A58" s="12" t="s">
         <v>54</v>
       </c>
@@ -12970,7 +12972,7 @@
       </c>
       <c r="E58" s="12"/>
     </row>
-    <row r="59" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" ht="15.75">
       <c r="A59" s="12" t="s">
         <v>55</v>
       </c>
@@ -12985,7 +12987,7 @@
       </c>
       <c r="E59" s="12"/>
     </row>
-    <row r="60" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="15.75">
       <c r="A60" s="12" t="s">
         <v>56</v>
       </c>
@@ -13000,7 +13002,7 @@
       </c>
       <c r="E60" s="12"/>
     </row>
-    <row r="61" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" ht="15.75">
       <c r="A61" s="12" t="s">
         <v>57</v>
       </c>
@@ -13017,7 +13019,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" ht="15.75">
       <c r="A62" s="12" t="s">
         <v>58</v>
       </c>
@@ -13034,7 +13036,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" ht="15.75">
       <c r="A63" s="12" t="s">
         <v>59</v>
       </c>
@@ -13051,7 +13053,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" ht="15.75">
       <c r="A64" s="12" t="s">
         <v>60</v>
       </c>
@@ -13068,7 +13070,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="15.75">
       <c r="A65" s="12" t="s">
         <v>61</v>
       </c>
@@ -13083,7 +13085,7 @@
       </c>
       <c r="E65" s="12"/>
     </row>
-    <row r="66" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" ht="15.75">
       <c r="A66" s="12" t="s">
         <v>62</v>
       </c>
@@ -13098,7 +13100,7 @@
       </c>
       <c r="E66" s="12"/>
     </row>
-    <row r="67" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" ht="15.75">
       <c r="A67" s="12" t="s">
         <v>63</v>
       </c>
@@ -13113,7 +13115,7 @@
       </c>
       <c r="E67" s="12"/>
     </row>
-    <row r="68" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" ht="15.75">
       <c r="A68" s="12" t="s">
         <v>64</v>
       </c>
@@ -13128,7 +13130,7 @@
       </c>
       <c r="E68" s="12"/>
     </row>
-    <row r="69" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" ht="15.75">
       <c r="A69" s="12" t="s">
         <v>65</v>
       </c>
@@ -13143,7 +13145,7 @@
       </c>
       <c r="E69" s="12"/>
     </row>
-    <row r="70" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" ht="15.75">
       <c r="A70" s="12" t="s">
         <v>66</v>
       </c>
@@ -13160,7 +13162,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" ht="15.75">
       <c r="A71" s="12" t="s">
         <v>67</v>
       </c>
@@ -13177,7 +13179,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" ht="15.75">
       <c r="A72" s="12" t="s">
         <v>68</v>
       </c>
@@ -13194,7 +13196,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" ht="15.75">
       <c r="A73" s="12" t="s">
         <v>69</v>
       </c>
@@ -13211,7 +13213,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" ht="15.75">
       <c r="A74" s="12" t="s">
         <v>70</v>
       </c>
@@ -13226,7 +13228,7 @@
       </c>
       <c r="E74" s="12"/>
     </row>
-    <row r="75" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="15.75">
       <c r="A75" s="12" t="s">
         <v>71</v>
       </c>
@@ -13241,7 +13243,7 @@
       </c>
       <c r="E75" s="12"/>
     </row>
-    <row r="76" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" ht="15.75">
       <c r="A76" s="12" t="s">
         <v>72</v>
       </c>
@@ -13256,7 +13258,7 @@
       </c>
       <c r="E76" s="12"/>
     </row>
-    <row r="77" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" ht="15.75">
       <c r="A77" s="12" t="s">
         <v>73</v>
       </c>
@@ -13271,7 +13273,7 @@
       </c>
       <c r="E77" s="12"/>
     </row>
-    <row r="78" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" ht="15.75">
       <c r="A78" s="12" t="s">
         <v>74</v>
       </c>
@@ -13286,7 +13288,7 @@
       </c>
       <c r="E78" s="12"/>
     </row>
-    <row r="79" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" ht="15.75">
       <c r="A79" s="12" t="s">
         <v>75</v>
       </c>
@@ -13303,7 +13305,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" ht="15.75">
       <c r="A80" s="12" t="s">
         <v>76</v>
       </c>
@@ -13320,7 +13322,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" ht="15.75">
       <c r="A81" s="12" t="s">
         <v>77</v>
       </c>
@@ -13337,7 +13339,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" ht="15.75">
       <c r="A82" s="12" t="s">
         <v>78</v>
       </c>
@@ -13354,7 +13356,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" ht="15.75">
       <c r="A83" s="12" t="s">
         <v>79</v>
       </c>
@@ -13369,7 +13371,7 @@
       </c>
       <c r="E83" s="12"/>
     </row>
-    <row r="84" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="15.75">
       <c r="A84" s="12" t="s">
         <v>80</v>
       </c>
@@ -13384,7 +13386,7 @@
       </c>
       <c r="E84" s="12"/>
     </row>
-    <row r="85" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" ht="15.75">
       <c r="A85" s="12" t="s">
         <v>81</v>
       </c>
@@ -13399,7 +13401,7 @@
       </c>
       <c r="E85" s="12"/>
     </row>
-    <row r="86" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" ht="15.75">
       <c r="A86" s="12" t="s">
         <v>82</v>
       </c>
@@ -13414,7 +13416,7 @@
       </c>
       <c r="E86" s="12"/>
     </row>
-    <row r="87" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" ht="15.75">
       <c r="A87" s="12" t="s">
         <v>83</v>
       </c>
@@ -13429,7 +13431,7 @@
       </c>
       <c r="E87" s="12"/>
     </row>
-    <row r="88" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" ht="15.75">
       <c r="A88" s="12" t="s">
         <v>84</v>
       </c>
@@ -13446,7 +13448,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" ht="15.75">
       <c r="A89" s="12" t="s">
         <v>85</v>
       </c>
@@ -13463,7 +13465,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" ht="15.75">
       <c r="A90" s="12" t="s">
         <v>86</v>
       </c>
@@ -13480,7 +13482,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" ht="15.75">
       <c r="A91" s="12" t="s">
         <v>87</v>
       </c>
@@ -13497,7 +13499,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" ht="15.75">
       <c r="A92" s="12" t="s">
         <v>88</v>
       </c>
@@ -13514,7 +13516,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" ht="15.75">
       <c r="A93" s="12" t="s">
         <v>89</v>
       </c>
@@ -13531,7 +13533,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" ht="15.75">
       <c r="A94" s="12" t="s">
         <v>90</v>
       </c>
@@ -13548,7 +13550,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" ht="15.75">
       <c r="A95" s="12" t="s">
         <v>91</v>
       </c>
@@ -13565,7 +13567,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" ht="15.75">
       <c r="A96" s="12" t="s">
         <v>92</v>
       </c>
@@ -13582,7 +13584,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" ht="15.75">
       <c r="A97" s="12" t="s">
         <v>93</v>
       </c>
@@ -13599,7 +13601,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" ht="15.75">
       <c r="A98" s="12" t="s">
         <v>94</v>
       </c>
@@ -13616,7 +13618,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" ht="15.75">
       <c r="A99" s="12" t="s">
         <v>95</v>
       </c>
@@ -13633,7 +13635,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" ht="15.75">
       <c r="A100" s="12" t="s">
         <v>96</v>
       </c>

</xml_diff>